<commit_message>
Added FPC interface board mapping xls
</commit_message>
<xml_diff>
--- a/docs/TPCape_RevA_BOM.xlsx
+++ b/docs/TPCape_RevA_BOM.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="9390" windowHeight="11655" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="9390" windowHeight="11655" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TPcape_BOM" sheetId="4" r:id="rId1"/>
     <sheet name="Connectors" sheetId="5" r:id="rId2"/>
+    <sheet name="interface" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725" iterate="1" iterateCount="10000"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="222">
   <si>
     <t>Capture CIS Standard Bill Of Materials - Standard Report</t>
   </si>
@@ -466,6 +467,222 @@
   </si>
   <si>
     <t>pru1_r30_13</t>
+  </si>
+  <si>
+    <t>P9.31</t>
+  </si>
+  <si>
+    <t>P9.29</t>
+  </si>
+  <si>
+    <t>P9.30</t>
+  </si>
+  <si>
+    <t>P9.28</t>
+  </si>
+  <si>
+    <t>P8.45</t>
+  </si>
+  <si>
+    <t>P8.46</t>
+  </si>
+  <si>
+    <t>P8.44</t>
+  </si>
+  <si>
+    <t>P8.43</t>
+  </si>
+  <si>
+    <t>pru0_r31_14</t>
+  </si>
+  <si>
+    <t>pru0_r31_15</t>
+  </si>
+  <si>
+    <t>pru0_r31_16</t>
+  </si>
+  <si>
+    <t>pru1_r31_16</t>
+  </si>
+  <si>
+    <t>SW</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>P8.41</t>
+  </si>
+  <si>
+    <t>P8.42</t>
+  </si>
+  <si>
+    <t>P8.39</t>
+  </si>
+  <si>
+    <t>P8.40</t>
+  </si>
+  <si>
+    <t>P9.6</t>
+  </si>
+  <si>
+    <t>P9.4</t>
+  </si>
+  <si>
+    <t>P9.42</t>
+  </si>
+  <si>
+    <t>P9.27</t>
+  </si>
+  <si>
+    <t>P9.41</t>
+  </si>
+  <si>
+    <t>P9.25</t>
+  </si>
+  <si>
+    <t>P8.30</t>
+  </si>
+  <si>
+    <t>P8.21</t>
+  </si>
+  <si>
+    <t>P8.20</t>
+  </si>
+  <si>
+    <t>P8.12</t>
+  </si>
+  <si>
+    <t>P8.11</t>
+  </si>
+  <si>
+    <t>P8.16</t>
+  </si>
+  <si>
+    <t>P8.15</t>
+  </si>
+  <si>
+    <t>P9.24</t>
+  </si>
+  <si>
+    <t>P9.26</t>
+  </si>
+  <si>
+    <t>Current limiting resistor for IF = 20mA (165-ohm for 3.3V, 90-ohm for 1.8V, 250-ohm for 5V)</t>
+  </si>
+  <si>
+    <t>Emitter resistor to GND, output to ADC?</t>
+  </si>
+  <si>
+    <t>VDD_5V</t>
+  </si>
+  <si>
+    <t>Tpcape</t>
+  </si>
+  <si>
+    <t>Vcc2</t>
+  </si>
+  <si>
+    <t>/PES</t>
+  </si>
+  <si>
+    <t>HUP</t>
+  </si>
+  <si>
+    <t>Vlog</t>
+  </si>
+  <si>
+    <t>HDO</t>
+  </si>
+  <si>
+    <t>HCLK</t>
+  </si>
+  <si>
+    <t>Vref</t>
+  </si>
+  <si>
+    <t>TMR2</t>
+  </si>
+  <si>
+    <t>/LAT</t>
+  </si>
+  <si>
+    <t>R35</t>
+  </si>
+  <si>
+    <t>CHOME</t>
+  </si>
+  <si>
+    <t>CSEL</t>
+  </si>
+  <si>
+    <t>MTA_2</t>
+  </si>
+  <si>
+    <t>MTAn_2</t>
+  </si>
+  <si>
+    <t>MTB_2</t>
+  </si>
+  <si>
+    <t>MTBn_2</t>
+  </si>
+  <si>
+    <t>1.8V for ADC? MOSFET to control for standby</t>
+  </si>
+  <si>
+    <t>Same as VSEN pin2 above</t>
+  </si>
+  <si>
+    <t>MCR10HJ181</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R33 (MCR01MZSF1502) emitter resistor to GND, C30 (GRM155B11H222KA01) decap, C37 (GRM1552C1H470JZ01) decap at MCU input, </t>
+  </si>
+  <si>
+    <t>C31 (GRM155F11C104ZA01) decap to AGND, MOSFET controlled by /HON</t>
+  </si>
+  <si>
+    <t>C33 (GRM155F11C104ZA01) decap to AGND, MOSFET controlled by /SRD</t>
+  </si>
+  <si>
+    <t>C34 (GRM155F11C104ZA01) decap to AGND</t>
+  </si>
+  <si>
+    <t>R31 (MCR01HJ102), R32 (MCR01HJ472), CA2 (GNM314B11H102KD01D) chatter prevention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA21 (MNR14E0ABJ223), CA3 (GNM314B11H102KD01D) </t>
+  </si>
+  <si>
+    <t>Connect to AGND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA24 (MNR14E0ABJ223), CA2 (GNM314B11H102KD01D) </t>
+  </si>
+  <si>
+    <t>RA23a (MNR14E0ABJ223), CA1 (GNM314B11H102KD01D)</t>
+  </si>
+  <si>
+    <t>C32 (GRM155B11H222KA01) to AGND, R28 (MCR01MZSF1002), C36 (GRM1552C1H470JZ01) decap to DGND at MCU, derived from Vcc and /HON</t>
+  </si>
+  <si>
+    <t>M14</t>
+  </si>
+  <si>
+    <t>M15</t>
+  </si>
+  <si>
+    <t>M14 (LB1936V-TLM-E), D4 (RB500V), D12 (RB500V), RA17 (MNR14E0ABJ223)</t>
+  </si>
+  <si>
+    <t>RA24 (MNR14E0ABJ223), CA1 (GNM314B11H102KD01D), JP18 (DNI) , Q7 (DTC124EUA), Q8 (DTA124EUA), Q9 (2SK2090-T1-A) circuit</t>
+  </si>
+  <si>
+    <t>R64 (MCR10HJ181), C59 (GRM155B11H222KA01)</t>
+  </si>
+  <si>
+    <t>R63 (MCR01MZSF1502), C58 (GRM155B11H222KA01), C40 (GRM1552C1H470JZ01) decap to DGND at MCU</t>
   </si>
 </sst>
 </file>
@@ -564,7 +781,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -576,7 +793,13 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1421,18 +1644,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.140625" customWidth="1"/>
     <col min="3" max="3" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="45.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1440,14 +1662,6 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="G2" t="s">
-        <v>135</v>
-      </c>
-      <c r="H2" t="s">
-        <v>139</v>
-      </c>
-    </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>68</v>
@@ -1467,177 +1681,155 @@
       <c r="F3" t="s">
         <v>73</v>
       </c>
-      <c r="G3" t="s">
-        <v>136</v>
-      </c>
-      <c r="H3" t="s">
-        <v>140</v>
-      </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="8">
+      <c r="A4" s="9">
         <v>1</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="D4" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>96</v>
+      </c>
       <c r="F4" t="s">
         <v>99</v>
       </c>
-      <c r="G4" t="s">
-        <v>134</v>
-      </c>
-      <c r="H4" t="s">
-        <v>141</v>
+      <c r="G4" s="10" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="8">
+      <c r="A5" s="9">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+      <c r="C5" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>128</v>
+      </c>
       <c r="F5" t="s">
         <v>100</v>
       </c>
-      <c r="G5" t="s">
-        <v>133</v>
-      </c>
-      <c r="H5" t="s">
-        <v>142</v>
+      <c r="G5" s="10" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="8">
+      <c r="A6" s="9">
         <v>3</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
       <c r="F6" t="s">
         <v>101</v>
       </c>
-      <c r="G6" t="s">
-        <v>130</v>
-      </c>
-      <c r="H6" t="s">
-        <v>143</v>
+      <c r="G6" s="10" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="8">
+      <c r="A7" s="9">
         <v>4</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8" t="s">
-        <v>84</v>
+      <c r="C7" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>185</v>
       </c>
       <c r="F7" t="s">
         <v>102</v>
       </c>
-      <c r="G7" t="s">
-        <v>131</v>
-      </c>
-      <c r="H7" t="s">
-        <v>144</v>
-      </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="8">
+      <c r="A8" s="9">
         <v>5</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8" t="s">
-        <v>84</v>
+      <c r="C8" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>185</v>
       </c>
       <c r="F8" t="s">
         <v>102</v>
       </c>
-      <c r="G8" t="s">
-        <v>132</v>
-      </c>
-      <c r="H8" t="s">
-        <v>145</v>
-      </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="8">
+      <c r="A9" s="9">
         <v>6</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+      <c r="C9" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="9"/>
       <c r="F9" t="s">
         <v>103</v>
       </c>
-      <c r="G9" t="s">
-        <v>129</v>
-      </c>
-      <c r="H9" t="s">
-        <v>146</v>
-      </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="8">
+      <c r="A10" s="9">
         <v>7</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="C10" s="9" t="s">
+        <v>97</v>
+      </c>
       <c r="F10" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="8">
+      <c r="A11" s="9">
         <v>8</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8" t="s">
+      <c r="D11" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>127</v>
       </c>
       <c r="F11" t="s">
@@ -1645,494 +1837,1840 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="8">
+      <c r="A12" s="9">
         <v>9</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8" t="s">
+      <c r="D12" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" s="9" t="s">
         <v>127</v>
       </c>
       <c r="F12" t="s">
         <v>105</v>
       </c>
+      <c r="G12" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="H12" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="8">
+      <c r="A13" s="9">
         <v>10</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
+      <c r="C13" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="E13" t="s">
+        <v>145</v>
+      </c>
       <c r="F13" t="s">
         <v>106</v>
       </c>
+      <c r="G13" s="9" t="s">
+        <v>174</v>
+      </c>
       <c r="H13" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="8">
+      <c r="A14" s="9">
         <v>11</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="C14" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="E14" t="s">
+        <v>144</v>
+      </c>
       <c r="F14" t="s">
         <v>107</v>
       </c>
+      <c r="G14" s="9" t="s">
+        <v>175</v>
+      </c>
       <c r="H14" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="8">
+      <c r="A15" s="9">
         <v>12</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="C15" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="E15" t="s">
+        <v>143</v>
+      </c>
       <c r="F15" t="s">
         <v>108</v>
       </c>
+      <c r="G15" s="9" t="s">
+        <v>176</v>
+      </c>
       <c r="H15" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="8">
+      <c r="A16" s="9">
         <v>13</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8" t="s">
+      <c r="C16" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="E16" s="9" t="s">
         <v>128</v>
       </c>
       <c r="F16" t="s">
         <v>112</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="H16" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="8">
+    <row r="17" spans="1:8">
+      <c r="A17" s="9">
         <v>14</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
       <c r="F17" t="s">
         <v>113</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="H17" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="8">
+    <row r="18" spans="1:8">
+      <c r="A18" s="9">
         <v>15</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
       <c r="F18" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="8">
+      <c r="G18" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="H18" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="9">
         <v>16</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="C19" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="E19" t="s">
+        <v>142</v>
+      </c>
       <c r="F19" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="8">
+      <c r="G19" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="H19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="9">
         <v>17</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="C20" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="E20" t="s">
+        <v>141</v>
+      </c>
       <c r="F20" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="8">
+      <c r="G20" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="H20" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="9">
         <v>18</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
+      <c r="C21" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E21" t="s">
+        <v>140</v>
+      </c>
       <c r="F21" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="8">
+      <c r="G21" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="H21" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="9">
         <v>19</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8" t="s">
+      <c r="D22" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" s="9" t="s">
         <v>127</v>
       </c>
       <c r="F22" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="8">
+    <row r="23" spans="1:8">
+      <c r="A23" s="9">
         <v>20</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8" t="s">
+      <c r="D23" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="9" t="s">
         <v>127</v>
       </c>
       <c r="F23" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="8">
+    <row r="24" spans="1:8">
+      <c r="A24" s="9">
         <v>21</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
+      <c r="C24" s="9" t="s">
+        <v>97</v>
+      </c>
       <c r="F24" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="8">
+    <row r="25" spans="1:8">
+      <c r="A25" s="9">
         <v>22</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
+      <c r="D25" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E25" t="s">
+        <v>146</v>
+      </c>
       <c r="F25" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="8">
+    <row r="26" spans="1:8">
+      <c r="A26" s="9">
         <v>23</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8" t="s">
-        <v>84</v>
+      <c r="C26" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>185</v>
       </c>
       <c r="F26" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="8">
+    <row r="27" spans="1:8">
+      <c r="A27" s="9">
         <v>24</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8" t="s">
-        <v>84</v>
+      <c r="C27" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>185</v>
       </c>
       <c r="F27" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="8">
+    <row r="28" spans="1:8">
+      <c r="A28" s="9">
         <v>25</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
+      <c r="C28" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="E28" s="9"/>
       <c r="F28" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="8">
+    <row r="29" spans="1:8">
+      <c r="A29" s="9">
         <v>26</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C29" s="8" t="s">
+      <c r="B29" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
       <c r="F29" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="8">
+    <row r="30" spans="1:8">
+      <c r="A30" s="9">
         <v>27</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
+      <c r="C30" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" t="s">
+        <v>151</v>
+      </c>
+      <c r="E30" t="s">
+        <v>136</v>
+      </c>
       <c r="F30" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="8">
+    <row r="31" spans="1:8">
+      <c r="A31" s="9">
         <v>28</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C31" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
+      <c r="C31" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" t="s">
+        <v>150</v>
+      </c>
+      <c r="E31" t="s">
+        <v>135</v>
+      </c>
       <c r="F31" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="8">
+    <row r="32" spans="1:8">
+      <c r="A32" s="9">
         <v>29</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C32" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
+      <c r="C32" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32" t="s">
+        <v>153</v>
+      </c>
+      <c r="E32" t="s">
+        <v>133</v>
+      </c>
       <c r="F32" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="8">
+    <row r="33" spans="1:7">
+      <c r="A33" s="9">
         <v>30</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C33" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
+      <c r="C33" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" t="s">
+        <v>152</v>
+      </c>
+      <c r="E33" t="s">
+        <v>134</v>
+      </c>
       <c r="F33" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="8">
+    <row r="36" spans="1:7">
+      <c r="A36" s="9">
         <v>1</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="8" t="s">
-        <v>97</v>
+      <c r="C36" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="F36" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="8">
+      <c r="G36" s="10" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="9">
         <v>2</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="9" t="s">
         <v>98</v>
       </c>
       <c r="F37" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="8">
+      <c r="G37" s="10" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="9">
         <v>3</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E38" s="9" t="s">
         <v>96</v>
       </c>
       <c r="F38" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="8">
+      <c r="G38" s="10" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="9">
         <v>4</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C39" s="8" t="s">
-        <v>97</v>
+      <c r="C39" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39" t="s">
+        <v>170</v>
+      </c>
+      <c r="E39" t="s">
+        <v>130</v>
       </c>
       <c r="F39" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="8">
+    <row r="40" spans="1:7">
+      <c r="A40" s="9">
         <v>5</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="C40" s="8" t="s">
-        <v>97</v>
+      <c r="C40" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D40" t="s">
+        <v>171</v>
+      </c>
+      <c r="E40" t="s">
+        <v>131</v>
       </c>
       <c r="F40" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="8">
+    <row r="41" spans="1:7">
+      <c r="A41" s="9">
         <v>6</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B41" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C41" s="8" t="s">
-        <v>97</v>
+      <c r="C41" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D41" t="s">
+        <v>172</v>
+      </c>
+      <c r="E41" t="s">
+        <v>132</v>
       </c>
       <c r="F41" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="8">
+    <row r="42" spans="1:7">
+      <c r="A42" s="9">
         <v>7</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C42" s="8" t="s">
-        <v>97</v>
+      <c r="C42" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E42" t="s">
+        <v>129</v>
       </c>
       <c r="F42" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="8">
+    <row r="43" spans="1:7">
+      <c r="A43" s="9">
         <v>8</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="9" t="s">
         <v>96</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:L43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="12" max="12" width="25.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:12">
+      <c r="B2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K3" t="s">
+        <v>70</v>
+      </c>
+      <c r="L3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" s="9">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>196</v>
+      </c>
+      <c r="G4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I4" s="9">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>196</v>
+      </c>
+      <c r="K4" t="s">
+        <v>96</v>
+      </c>
+      <c r="L4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" s="9">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>187</v>
+      </c>
+      <c r="G5" t="s">
+        <v>97</v>
+      </c>
+      <c r="I5" s="9">
+        <v>2</v>
+      </c>
+      <c r="J5" t="s">
+        <v>187</v>
+      </c>
+      <c r="K5" t="s">
+        <v>97</v>
+      </c>
+      <c r="L5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="9">
+        <v>3</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" s="9">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>188</v>
+      </c>
+      <c r="G6" t="s">
+        <v>98</v>
+      </c>
+      <c r="I6" s="9">
+        <v>3</v>
+      </c>
+      <c r="J6" t="s">
+        <v>188</v>
+      </c>
+      <c r="K6" t="s">
+        <v>98</v>
+      </c>
+      <c r="L6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="9">
+        <v>4</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" s="9">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" t="s">
+        <v>97</v>
+      </c>
+      <c r="I7" s="9">
+        <v>4</v>
+      </c>
+      <c r="J7" t="s">
+        <v>189</v>
+      </c>
+      <c r="K7" t="s">
+        <v>98</v>
+      </c>
+      <c r="L7" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="9">
+        <v>5</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="9">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G8" t="s">
+        <v>97</v>
+      </c>
+      <c r="I8" s="9">
+        <v>5</v>
+      </c>
+      <c r="J8" t="s">
+        <v>190</v>
+      </c>
+      <c r="K8" t="s">
+        <v>97</v>
+      </c>
+      <c r="L8" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9" s="9">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>191</v>
+      </c>
+      <c r="G9" t="s">
+        <v>97</v>
+      </c>
+      <c r="I9" s="9">
+        <v>6</v>
+      </c>
+      <c r="J9" t="s">
+        <v>77</v>
+      </c>
+      <c r="K9" t="s">
+        <v>97</v>
+      </c>
+      <c r="L9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="9">
+        <v>7</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="9">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>192</v>
+      </c>
+      <c r="G10" t="s">
+        <v>97</v>
+      </c>
+      <c r="I10" s="9">
+        <v>7</v>
+      </c>
+      <c r="J10" t="s">
+        <v>77</v>
+      </c>
+      <c r="K10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="9">
+        <v>8</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" s="9">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" t="s">
+        <v>96</v>
+      </c>
+      <c r="I11" s="9">
+        <v>8</v>
+      </c>
+      <c r="J11" t="s">
+        <v>191</v>
+      </c>
+      <c r="K11" t="s">
+        <v>97</v>
+      </c>
+      <c r="L11" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="9">
+        <v>9</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" s="9">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G12" t="s">
+        <v>96</v>
+      </c>
+      <c r="I12" s="9">
+        <v>9</v>
+      </c>
+      <c r="J12" t="s">
+        <v>192</v>
+      </c>
+      <c r="K12" t="s">
+        <v>97</v>
+      </c>
+      <c r="L12" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="9">
+        <v>10</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" s="9">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" t="s">
+        <v>97</v>
+      </c>
+      <c r="I13" s="9">
+        <v>10</v>
+      </c>
+      <c r="J13" t="s">
+        <v>80</v>
+      </c>
+      <c r="K13" t="s">
+        <v>96</v>
+      </c>
+      <c r="L13" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="9">
+        <v>11</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14" s="9">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>82</v>
+      </c>
+      <c r="G14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I14" s="9">
+        <v>11</v>
+      </c>
+      <c r="J14" t="s">
+        <v>80</v>
+      </c>
+      <c r="K14" t="s">
+        <v>96</v>
+      </c>
+      <c r="L14" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="9">
+        <v>12</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E15" s="9">
+        <v>14</v>
+      </c>
+      <c r="F15" t="s">
+        <v>83</v>
+      </c>
+      <c r="G15" t="s">
+        <v>97</v>
+      </c>
+      <c r="I15" s="9">
+        <v>12</v>
+      </c>
+      <c r="J15" t="s">
+        <v>81</v>
+      </c>
+      <c r="K15" t="s">
+        <v>97</v>
+      </c>
+      <c r="L15" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="9">
+        <v>13</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="9">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
+        <v>190</v>
+      </c>
+      <c r="G16" t="s">
+        <v>97</v>
+      </c>
+      <c r="I16" s="9">
+        <v>13</v>
+      </c>
+      <c r="J16" t="s">
+        <v>82</v>
+      </c>
+      <c r="K16" t="s">
+        <v>97</v>
+      </c>
+      <c r="L16" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="9">
+        <v>14</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" s="9">
+        <v>16</v>
+      </c>
+      <c r="F17" t="s">
+        <v>193</v>
+      </c>
+      <c r="I17" s="9">
+        <v>14</v>
+      </c>
+      <c r="J17" t="s">
+        <v>83</v>
+      </c>
+      <c r="K17" t="s">
+        <v>97</v>
+      </c>
+      <c r="L17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="9">
+        <v>15</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E18" s="9">
+        <v>17</v>
+      </c>
+      <c r="F18" t="s">
+        <v>194</v>
+      </c>
+      <c r="I18" s="9">
+        <v>15</v>
+      </c>
+      <c r="J18" t="s">
+        <v>190</v>
+      </c>
+      <c r="K18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="9">
+        <v>16</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19" s="9">
+        <v>18</v>
+      </c>
+      <c r="F19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" t="s">
+        <v>97</v>
+      </c>
+      <c r="I19" s="9">
+        <v>16</v>
+      </c>
+      <c r="J19" t="s">
+        <v>193</v>
+      </c>
+      <c r="L19" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="9">
+        <v>17</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20" s="9">
+        <v>19</v>
+      </c>
+      <c r="F20" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" t="s">
+        <v>97</v>
+      </c>
+      <c r="I20" s="9">
+        <v>17</v>
+      </c>
+      <c r="J20" t="s">
+        <v>194</v>
+      </c>
+      <c r="L20" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="9">
+        <v>18</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21" s="9">
+        <v>20</v>
+      </c>
+      <c r="F21" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" t="s">
+        <v>97</v>
+      </c>
+      <c r="I21" s="9">
+        <v>18</v>
+      </c>
+      <c r="J21" t="s">
+        <v>86</v>
+      </c>
+      <c r="K21" t="s">
+        <v>97</v>
+      </c>
+      <c r="L21" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="9">
+        <v>19</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" s="9">
+        <v>21</v>
+      </c>
+      <c r="F22" t="s">
+        <v>80</v>
+      </c>
+      <c r="G22" t="s">
+        <v>96</v>
+      </c>
+      <c r="I22" s="9">
+        <v>19</v>
+      </c>
+      <c r="J22" t="s">
+        <v>87</v>
+      </c>
+      <c r="K22" t="s">
+        <v>97</v>
+      </c>
+      <c r="L22" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="9">
+        <v>20</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="9">
+        <v>22</v>
+      </c>
+      <c r="F23" t="s">
+        <v>80</v>
+      </c>
+      <c r="G23" t="s">
+        <v>96</v>
+      </c>
+      <c r="I23" s="9">
+        <v>20</v>
+      </c>
+      <c r="J23" t="s">
+        <v>88</v>
+      </c>
+      <c r="K23" t="s">
+        <v>97</v>
+      </c>
+      <c r="L23" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="9">
+        <v>21</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24" s="9">
+        <v>23</v>
+      </c>
+      <c r="F24" t="s">
+        <v>195</v>
+      </c>
+      <c r="G24" t="s">
+        <v>97</v>
+      </c>
+      <c r="I24" s="9">
+        <v>21</v>
+      </c>
+      <c r="J24" t="s">
+        <v>80</v>
+      </c>
+      <c r="K24" t="s">
+        <v>96</v>
+      </c>
+      <c r="L24" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="9">
+        <v>22</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E25" s="9">
+        <v>24</v>
+      </c>
+      <c r="F25" t="s">
+        <v>78</v>
+      </c>
+      <c r="G25" t="s">
+        <v>98</v>
+      </c>
+      <c r="I25" s="9">
+        <v>22</v>
+      </c>
+      <c r="J25" t="s">
+        <v>80</v>
+      </c>
+      <c r="K25" t="s">
+        <v>96</v>
+      </c>
+      <c r="L25" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="9">
+        <v>23</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E26" s="9">
+        <v>25</v>
+      </c>
+      <c r="F26" t="s">
+        <v>77</v>
+      </c>
+      <c r="G26" t="s">
+        <v>97</v>
+      </c>
+      <c r="I26" s="9">
+        <v>23</v>
+      </c>
+      <c r="J26" t="s">
+        <v>195</v>
+      </c>
+      <c r="K26" t="s">
+        <v>97</v>
+      </c>
+      <c r="L26" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="9">
+        <v>24</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E27" s="9">
+        <v>26</v>
+      </c>
+      <c r="F27" t="s">
+        <v>77</v>
+      </c>
+      <c r="G27" t="s">
+        <v>97</v>
+      </c>
+      <c r="I27" s="9">
+        <v>24</v>
+      </c>
+      <c r="J27" t="s">
+        <v>78</v>
+      </c>
+      <c r="K27" t="s">
+        <v>98</v>
+      </c>
+      <c r="L27" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="9">
+        <v>25</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E28" s="9">
+        <v>5</v>
+      </c>
+      <c r="F28" t="s">
+        <v>190</v>
+      </c>
+      <c r="G28" t="s">
+        <v>97</v>
+      </c>
+      <c r="I28" s="9">
+        <v>25</v>
+      </c>
+      <c r="J28" t="s">
+        <v>77</v>
+      </c>
+      <c r="K28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="9">
+        <v>26</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E29" s="9">
+        <v>4</v>
+      </c>
+      <c r="F29" t="s">
+        <v>189</v>
+      </c>
+      <c r="G29" t="s">
+        <v>98</v>
+      </c>
+      <c r="I29" s="9">
+        <v>26</v>
+      </c>
+      <c r="J29" t="s">
+        <v>77</v>
+      </c>
+      <c r="K29" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="9">
+        <v>27</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E30" s="9">
+        <v>27</v>
+      </c>
+      <c r="F30" t="s">
+        <v>92</v>
+      </c>
+      <c r="G30" t="s">
+        <v>97</v>
+      </c>
+      <c r="I30" s="9">
+        <v>27</v>
+      </c>
+      <c r="J30" t="s">
+        <v>92</v>
+      </c>
+      <c r="K30" t="s">
+        <v>97</v>
+      </c>
+      <c r="L30" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="9">
+        <v>28</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E31" s="9">
+        <v>28</v>
+      </c>
+      <c r="F31" t="s">
+        <v>93</v>
+      </c>
+      <c r="G31" t="s">
+        <v>97</v>
+      </c>
+      <c r="I31" s="9">
+        <v>28</v>
+      </c>
+      <c r="J31" t="s">
+        <v>93</v>
+      </c>
+      <c r="K31" t="s">
+        <v>97</v>
+      </c>
+      <c r="L31" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="9">
+        <v>29</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E32" s="9">
+        <v>29</v>
+      </c>
+      <c r="F32" t="s">
+        <v>94</v>
+      </c>
+      <c r="G32" t="s">
+        <v>97</v>
+      </c>
+      <c r="I32" s="9">
+        <v>29</v>
+      </c>
+      <c r="J32" t="s">
+        <v>94</v>
+      </c>
+      <c r="K32" t="s">
+        <v>97</v>
+      </c>
+      <c r="L32" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="9">
+        <v>30</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E33" s="9">
+        <v>30</v>
+      </c>
+      <c r="F33" t="s">
+        <v>95</v>
+      </c>
+      <c r="G33" t="s">
+        <v>97</v>
+      </c>
+      <c r="I33" s="9">
+        <v>30</v>
+      </c>
+      <c r="J33" t="s">
+        <v>95</v>
+      </c>
+      <c r="K33" t="s">
+        <v>97</v>
+      </c>
+      <c r="L33" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="9">
+        <v>1</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E36" s="9">
+        <v>1</v>
+      </c>
+      <c r="F36" t="s">
+        <v>187</v>
+      </c>
+      <c r="G36" t="s">
+        <v>97</v>
+      </c>
+      <c r="I36" s="9">
+        <v>1</v>
+      </c>
+      <c r="J36" t="s">
+        <v>187</v>
+      </c>
+      <c r="K36" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="9">
+        <v>2</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I37" s="9">
+        <v>2</v>
+      </c>
+      <c r="J37" t="s">
+        <v>197</v>
+      </c>
+      <c r="K37" t="s">
+        <v>98</v>
+      </c>
+      <c r="L37" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="9">
+        <v>3</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="I38" s="9">
+        <v>3</v>
+      </c>
+      <c r="J38" t="s">
+        <v>198</v>
+      </c>
+      <c r="K38" t="s">
+        <v>98</v>
+      </c>
+      <c r="L38" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="9">
+        <v>4</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E39" s="9">
+        <v>4</v>
+      </c>
+      <c r="F39" t="s">
+        <v>199</v>
+      </c>
+      <c r="G39" t="s">
+        <v>97</v>
+      </c>
+      <c r="I39" s="9">
+        <v>4</v>
+      </c>
+      <c r="J39" t="s">
+        <v>199</v>
+      </c>
+      <c r="K39" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="9">
+        <v>5</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E40" s="9">
+        <v>5</v>
+      </c>
+      <c r="F40" t="s">
+        <v>200</v>
+      </c>
+      <c r="G40" t="s">
+        <v>97</v>
+      </c>
+      <c r="I40" s="9">
+        <v>5</v>
+      </c>
+      <c r="J40" t="s">
+        <v>200</v>
+      </c>
+      <c r="K40" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="9">
+        <v>6</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E41" s="9">
+        <v>6</v>
+      </c>
+      <c r="F41" t="s">
+        <v>201</v>
+      </c>
+      <c r="G41" t="s">
+        <v>97</v>
+      </c>
+      <c r="I41" s="9">
+        <v>6</v>
+      </c>
+      <c r="J41" t="s">
+        <v>201</v>
+      </c>
+      <c r="K41" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="9">
+        <v>7</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E42" s="9">
+        <v>7</v>
+      </c>
+      <c r="F42" t="s">
+        <v>202</v>
+      </c>
+      <c r="G42" t="s">
+        <v>97</v>
+      </c>
+      <c r="I42" s="9">
+        <v>7</v>
+      </c>
+      <c r="J42" t="s">
+        <v>202</v>
+      </c>
+      <c r="K42" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="9">
+        <v>8</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="I43" s="9">
+        <v>8</v>
+      </c>
+      <c r="J43" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
3 versions init commit
</commit_message>
<xml_diff>
--- a/docs/TPCape_RevA_BOM.xlsx
+++ b/docs/TPCape_RevA_BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="9390" windowHeight="11655" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="9390" windowHeight="11655"/>
   </bookViews>
   <sheets>
     <sheet name="TPcape_BOM" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="259">
   <si>
     <t>Capture CIS Standard Bill Of Materials - Standard Report</t>
   </si>
@@ -683,6 +683,117 @@
   </si>
   <si>
     <t>R63 (MCR01MZSF1502), C58 (GRM155B11H222KA01), C40 (GRM1552C1H470JZ01) decap to DGND at MCU</t>
+  </si>
+  <si>
+    <t>GRM155F11C104ZA01</t>
+  </si>
+  <si>
+    <t>Murata</t>
+  </si>
+  <si>
+    <t>0.1uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0402, 16Vdc, </t>
+  </si>
+  <si>
+    <t>C31, C33, C34</t>
+  </si>
+  <si>
+    <t>MCR01MZSF1502</t>
+  </si>
+  <si>
+    <t>GRM155B11H222KA01</t>
+  </si>
+  <si>
+    <t>GRM1552C1H470JZ01</t>
+  </si>
+  <si>
+    <t>MCR01HJ102</t>
+  </si>
+  <si>
+    <t>R31</t>
+  </si>
+  <si>
+    <t>MCR01HJ472</t>
+  </si>
+  <si>
+    <t>R32</t>
+  </si>
+  <si>
+    <t>GNM314B11H102KD01D</t>
+  </si>
+  <si>
+    <t>MNR14E0ABJ223</t>
+  </si>
+  <si>
+    <t>CA1, CA2, CA3</t>
+  </si>
+  <si>
+    <t>C30, C32, C58, C59</t>
+  </si>
+  <si>
+    <t>R28</t>
+  </si>
+  <si>
+    <t>MCR01MZSF1002</t>
+  </si>
+  <si>
+    <t>C36, C37, C40</t>
+  </si>
+  <si>
+    <t>RA17, RA21, RA23a, RA24</t>
+  </si>
+  <si>
+    <t>DTC124EUA</t>
+  </si>
+  <si>
+    <t>Q7</t>
+  </si>
+  <si>
+    <t>R64</t>
+  </si>
+  <si>
+    <t>Rohm</t>
+  </si>
+  <si>
+    <t>Surface Mount Thick Film Chip Resistor 0402 Case 15K Ohms 1% Tolerance 100 PPM</t>
+  </si>
+  <si>
+    <t>15K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0402, 50Vdc, </t>
+  </si>
+  <si>
+    <t>2200pF</t>
+  </si>
+  <si>
+    <t>47pF</t>
+  </si>
+  <si>
+    <t>0402, 50Vdc, 0+/-60ppm/C</t>
+  </si>
+  <si>
+    <t>Surface Mount Thick Film Chip Resistor 0402 Case 10K Ohms 1% Tolerance 100 PPM</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>R33, R63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0603 x 4, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0402, 5%, </t>
+  </si>
+  <si>
+    <t>0402, 5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0805, 5%, </t>
   </si>
 </sst>
 </file>
@@ -693,7 +804,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="g"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -723,6 +834,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -781,7 +898,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -801,6 +918,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1097,10 +1215,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1417,7 +1535,7 @@
         <v>60</v>
       </c>
       <c r="L15" s="6">
-        <f>K15*B33</f>
+        <f>K15*B43</f>
         <v>0</v>
       </c>
     </row>
@@ -1524,6 +1642,12 @@
       <c r="A25" s="1">
         <v>17</v>
       </c>
+      <c r="C25" t="s">
+        <v>236</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>234</v>
+      </c>
       <c r="L25" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1542,6 +1666,21 @@
       <c r="A27" s="1">
         <v>19</v>
       </c>
+      <c r="C27" t="s">
+        <v>237</v>
+      </c>
+      <c r="D27" t="s">
+        <v>249</v>
+      </c>
+      <c r="E27" t="s">
+        <v>248</v>
+      </c>
+      <c r="F27" t="s">
+        <v>223</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>228</v>
+      </c>
       <c r="L27" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1551,6 +1690,21 @@
       <c r="A28" s="1">
         <v>20</v>
       </c>
+      <c r="C28" t="s">
+        <v>226</v>
+      </c>
+      <c r="D28" t="s">
+        <v>224</v>
+      </c>
+      <c r="E28" t="s">
+        <v>225</v>
+      </c>
+      <c r="F28" t="s">
+        <v>223</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>222</v>
+      </c>
       <c r="L28" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1560,6 +1714,21 @@
       <c r="A29" s="1">
         <v>21</v>
       </c>
+      <c r="C29" t="s">
+        <v>240</v>
+      </c>
+      <c r="D29" t="s">
+        <v>250</v>
+      </c>
+      <c r="E29" t="s">
+        <v>251</v>
+      </c>
+      <c r="F29" t="s">
+        <v>223</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>229</v>
+      </c>
       <c r="L29" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1587,6 +1756,21 @@
       <c r="A32" s="1">
         <v>24</v>
       </c>
+      <c r="C32" t="s">
+        <v>238</v>
+      </c>
+      <c r="D32" t="s">
+        <v>253</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="F32" t="s">
+        <v>245</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>239</v>
+      </c>
       <c r="L32" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1596,41 +1780,160 @@
       <c r="A33" s="1">
         <v>25</v>
       </c>
-      <c r="B33" s="1">
+      <c r="C33" t="s">
+        <v>231</v>
+      </c>
+      <c r="E33" t="s">
+        <v>256</v>
+      </c>
+      <c r="F33" t="s">
+        <v>245</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="1">
+        <v>26</v>
+      </c>
+      <c r="C34" t="s">
+        <v>233</v>
+      </c>
+      <c r="E34" t="s">
+        <v>257</v>
+      </c>
+      <c r="F34" t="s">
+        <v>245</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="1">
+        <v>27</v>
+      </c>
+      <c r="C35" t="s">
+        <v>254</v>
+      </c>
+      <c r="D35" t="s">
+        <v>247</v>
+      </c>
+      <c r="E35" t="s">
         <v>246</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="F35" t="s">
+        <v>245</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="1">
+        <v>28</v>
+      </c>
+      <c r="C36" t="s">
+        <v>244</v>
+      </c>
+      <c r="E36" t="s">
+        <v>258</v>
+      </c>
+      <c r="F36" t="s">
+        <v>245</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="1">
+        <v>29</v>
+      </c>
+      <c r="C37" t="s">
+        <v>241</v>
+      </c>
+      <c r="E37" t="s">
+        <v>255</v>
+      </c>
+      <c r="F37" t="s">
+        <v>245</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="1">
+        <v>31</v>
+      </c>
+      <c r="C39" t="s">
+        <v>243</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="1">
+        <v>25</v>
+      </c>
+      <c r="B43" s="1">
+        <v>246</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G43" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="H43" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I33" s="2" t="s">
+      <c r="I43" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J33" s="4" t="s">
+      <c r="J43" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="L33" s="6" t="e">
-        <f>K33*#REF!</f>
+      <c r="L43" s="6" t="e">
+        <f>K43*#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J33" r:id="rId1"/>
+    <hyperlink ref="J43" r:id="rId1"/>
     <hyperlink ref="J12" r:id="rId2"/>
     <hyperlink ref="J11" r:id="rId3"/>
     <hyperlink ref="J14" r:id="rId4"/>
@@ -2479,8 +2782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Added EEPROM and power research
</commit_message>
<xml_diff>
--- a/docs/TPCape_RevA_BOM.xlsx
+++ b/docs/TPCape_RevA_BOM.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\thermal-printer\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="9390" windowHeight="11655" activeTab="1"/>
   </bookViews>
@@ -17,12 +12,12 @@
     <sheet name="interface" sheetId="6" r:id="rId3"/>
     <sheet name="motor" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511" iterate="1" iterateCount="10000"/>
+  <calcPr calcId="125725" iterate="1" iterateCount="10000"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="293">
   <si>
     <t>Capture CIS Standard Bill Of Materials - Standard Report</t>
   </si>
@@ -645,9 +640,6 @@
     <t xml:space="preserve">R33 (MCR01MZSF1502) emitter resistor to GND, C30 (GRM155B11H222KA01) decap, C37 (GRM1552C1H470JZ01) decap at MCU input, </t>
   </si>
   <si>
-    <t>C31 (GRM155F11C104ZA01) decap to AGND, MOSFET controlled by /HON</t>
-  </si>
-  <si>
     <t>C33 (GRM155F11C104ZA01) decap to AGND, MOSFET controlled by /SRD</t>
   </si>
   <si>
@@ -847,17 +839,74 @@
   </si>
   <si>
     <t>nfault</t>
+  </si>
+  <si>
+    <t>C1, C2</t>
+  </si>
+  <si>
+    <t>UWT1C470MBL1GB</t>
+  </si>
+  <si>
+    <t>Nichicon</t>
+  </si>
+  <si>
+    <t>C31 (GRM155F11C104ZA01) decap to AGND, MOSFET controlled by /HON, C2 at CN7 input</t>
+  </si>
+  <si>
+    <t>RA24 (MNR14E0ABJ223), CA2 (GNM314B11H102KD01D), C1 decap at CN7 input</t>
+  </si>
+  <si>
+    <t>47uF</t>
+  </si>
+  <si>
+    <t>Aluminum electrolytic cap, 16V, 20%, 6.3x5.4</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>MMC1_CLK</t>
+  </si>
+  <si>
+    <t>MMC1_CMD</t>
+  </si>
+  <si>
+    <t>CAT24C256WI-GT3</t>
+  </si>
+  <si>
+    <t>ON Semi</t>
+  </si>
+  <si>
+    <t>CAT24C256WI-GT3OSCT-ND</t>
+  </si>
+  <si>
+    <t>IC EEPROM 256KBIT 400KHZ 8SOIC</t>
+  </si>
+  <si>
+    <t>~1.46V (PWM @ 5V)</t>
+  </si>
+  <si>
+    <t>~1.46V (PWM @ 5V) at standby. 5V running</t>
+  </si>
+  <si>
+    <t>Outputs 0 if no paper. Outputs ~0.85V (PWM @ 5V) if paper detected, or 5V when running</t>
+  </si>
+  <si>
+    <t>head signal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="g"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -892,6 +941,12 @@
       <sz val="9"/>
       <color rgb="FF3F3F3F"/>
       <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -951,7 +1006,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -972,6 +1027,8 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1034,7 +1091,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1066,10 +1123,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1101,7 +1157,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1277,14 +1332,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.42578125" customWidth="1"/>
     <col min="2" max="2" width="4.5703125" bestFit="1" customWidth="1"/>
@@ -1301,7 +1356,7 @@
     <col min="13" max="13" width="62.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1311,7 +1366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1322,27 +1377,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1383,7 +1438,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -1410,7 +1465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -1437,7 +1492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="1">
         <v>3</v>
       </c>
@@ -1476,7 +1531,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="1">
         <v>4</v>
       </c>
@@ -1515,7 +1570,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" s="1">
         <v>5</v>
       </c>
@@ -1544,7 +1599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" s="1">
         <v>6</v>
       </c>
@@ -1584,7 +1639,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" s="1">
         <v>7</v>
       </c>
@@ -1602,7 +1657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" s="1">
         <v>8</v>
       </c>
@@ -1620,7 +1675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="A17" s="1">
         <v>9</v>
       </c>
@@ -1638,7 +1693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" s="1">
         <v>10</v>
       </c>
@@ -1647,16 +1702,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" s="1">
         <v>11</v>
       </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="I19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="K19" s="6">
+        <v>0.73</v>
+      </c>
       <c r="L19" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="1">
         <v>12</v>
       </c>
@@ -1665,7 +1741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21" s="1">
         <v>13</v>
       </c>
@@ -1674,7 +1750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" s="1">
         <v>14</v>
       </c>
@@ -1683,7 +1759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23" s="1">
         <v>15</v>
       </c>
@@ -1692,7 +1768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="A24" s="1">
         <v>16</v>
       </c>
@@ -1701,103 +1777,118 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12">
       <c r="A25" s="1">
         <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L25" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26" s="1">
         <v>18</v>
       </c>
+      <c r="C26" t="s">
+        <v>274</v>
+      </c>
+      <c r="D26" t="s">
+        <v>279</v>
+      </c>
+      <c r="E26" t="s">
+        <v>280</v>
+      </c>
+      <c r="F26" t="s">
+        <v>276</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>275</v>
+      </c>
       <c r="L26" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="A27" s="1">
         <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D27" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E27" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F27" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L27" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12">
       <c r="A28" s="1">
         <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D28" t="s">
+        <v>223</v>
+      </c>
+      <c r="E28" t="s">
         <v>224</v>
       </c>
-      <c r="E28" t="s">
-        <v>225</v>
-      </c>
       <c r="F28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="L28" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12">
       <c r="A29" s="1">
         <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D29" t="s">
+        <v>249</v>
+      </c>
+      <c r="E29" t="s">
         <v>250</v>
       </c>
-      <c r="E29" t="s">
-        <v>251</v>
-      </c>
       <c r="F29" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L29" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12">
       <c r="A30" s="1">
         <v>22</v>
       </c>
@@ -1806,7 +1897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12">
       <c r="A31" s="1">
         <v>23</v>
       </c>
@@ -1815,150 +1906,150 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12">
       <c r="A32" s="1">
         <v>24</v>
       </c>
       <c r="C32" t="s">
+        <v>237</v>
+      </c>
+      <c r="D32" t="s">
+        <v>252</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="F32" t="s">
+        <v>244</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="D32" t="s">
-        <v>253</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="F32" t="s">
-        <v>245</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>239</v>
       </c>
       <c r="L32" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12">
       <c r="A33" s="1">
         <v>25</v>
       </c>
       <c r="C33" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E33" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F33" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" s="1">
         <v>26</v>
       </c>
       <c r="C34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E34" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F34" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" s="1">
         <v>27</v>
       </c>
       <c r="C35" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D35" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E35" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F35" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" s="1">
         <v>28</v>
       </c>
       <c r="C36" t="s">
+        <v>243</v>
+      </c>
+      <c r="E36" t="s">
+        <v>257</v>
+      </c>
+      <c r="F36" t="s">
         <v>244</v>
-      </c>
-      <c r="E36" t="s">
-        <v>258</v>
-      </c>
-      <c r="F36" t="s">
-        <v>245</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12">
       <c r="A37" s="1">
         <v>29</v>
       </c>
       <c r="C37" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F37" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12">
       <c r="A39" s="1">
         <v>31</v>
       </c>
       <c r="C39" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12">
       <c r="A41" s="1">
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12">
       <c r="A42" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12">
       <c r="A43" s="1">
         <v>25</v>
       </c>
@@ -2000,21 +2091,23 @@
     <hyperlink ref="J12" r:id="rId2"/>
     <hyperlink ref="J11" r:id="rId3"/>
     <hyperlink ref="J14" r:id="rId4"/>
+    <hyperlink ref="G19" r:id="rId5" display="https://www.onsemi.com/PowerSolutions/product.do?id=CAT24C256WI-GT3"/>
+    <hyperlink ref="J19" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.140625" customWidth="1"/>
     <col min="3" max="3" width="3.85546875" bestFit="1" customWidth="1"/>
@@ -2023,12 +2116,12 @@
     <col min="7" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -2048,7 +2141,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -2071,7 +2164,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -2094,7 +2187,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -2113,7 +2206,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -2133,7 +2226,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -2153,7 +2246,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" s="9">
         <v>6</v>
       </c>
@@ -2168,7 +2261,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="9">
         <v>7</v>
       </c>
@@ -2182,7 +2275,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" s="9">
         <v>8</v>
       </c>
@@ -2202,7 +2295,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" s="9">
         <v>9</v>
       </c>
@@ -2228,7 +2321,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" s="9">
         <v>10</v>
       </c>
@@ -2254,7 +2347,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="9">
         <v>11</v>
       </c>
@@ -2279,8 +2372,11 @@
       <c r="H14" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="9">
         <v>12</v>
       </c>
@@ -2305,8 +2401,11 @@
       <c r="H15" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="9">
         <v>13</v>
       </c>
@@ -2332,7 +2431,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="9">
         <v>14</v>
       </c>
@@ -2354,7 +2453,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="9">
         <v>15</v>
       </c>
@@ -2376,7 +2475,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="9">
         <v>16</v>
       </c>
@@ -2402,7 +2501,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="9">
         <v>17</v>
       </c>
@@ -2428,7 +2527,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="9">
         <v>18</v>
       </c>
@@ -2454,7 +2553,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="9">
         <v>19</v>
       </c>
@@ -2474,7 +2573,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="9">
         <v>20</v>
       </c>
@@ -2494,7 +2593,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" s="9">
         <v>21</v>
       </c>
@@ -2508,7 +2607,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="9">
         <v>22</v>
       </c>
@@ -2528,7 +2627,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="9">
         <v>23</v>
       </c>
@@ -2548,7 +2647,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="9">
         <v>24</v>
       </c>
@@ -2568,7 +2667,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="9">
         <v>25</v>
       </c>
@@ -2586,7 +2685,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="9">
         <v>26</v>
       </c>
@@ -2602,7 +2701,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="9">
         <v>27</v>
       </c>
@@ -2622,7 +2721,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="9">
         <v>28</v>
       </c>
@@ -2642,7 +2741,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="9">
         <v>29</v>
       </c>
@@ -2662,7 +2761,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" s="9">
         <v>30</v>
       </c>
@@ -2682,7 +2781,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="A36" s="9">
         <v>1</v>
       </c>
@@ -2705,7 +2804,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7">
       <c r="A37" s="9">
         <v>2</v>
       </c>
@@ -2722,7 +2821,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7">
       <c r="A38" s="9">
         <v>3</v>
       </c>
@@ -2745,7 +2844,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7">
       <c r="A39" s="9">
         <v>4</v>
       </c>
@@ -2765,7 +2864,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7">
       <c r="A40" s="9">
         <v>5</v>
       </c>
@@ -2785,7 +2884,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7">
       <c r="A41" s="9">
         <v>6</v>
       </c>
@@ -2805,7 +2904,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7">
       <c r="A42" s="9">
         <v>7</v>
       </c>
@@ -2825,7 +2924,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7">
       <c r="A43" s="9">
         <v>8</v>
       </c>
@@ -2836,66 +2935,98 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7">
       <c r="A47">
         <v>6</v>
       </c>
       <c r="B47" t="s">
+        <v>267</v>
+      </c>
+      <c r="E47" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48">
+        <v>3</v>
+      </c>
+      <c r="B48" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>4</v>
-      </c>
-      <c r="B48" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49">
         <v>4</v>
       </c>
       <c r="B49" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+      <c r="E49" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50">
         <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+      <c r="E50" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51" t="s">
+        <v>292</v>
+      </c>
+      <c r="E51" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52">
         <v>2</v>
-      </c>
-      <c r="B51" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>1</v>
       </c>
       <c r="B52" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B53" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <f>SUM(A47:A53)</f>
-        <v>22</v>
+        <v>271</v>
+      </c>
+      <c r="E53" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54" t="s">
+        <v>272</v>
+      </c>
+      <c r="E54" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56">
+        <f>SUM(A47:A52)</f>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2904,24 +3035,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:M43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="12" max="12" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="B2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -2953,7 +3084,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -2985,7 +3116,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -3014,10 +3145,13 @@
         <v>97</v>
       </c>
       <c r="L5" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="M5" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -3048,8 +3182,11 @@
       <c r="L6" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -3078,10 +3215,10 @@
         <v>98</v>
       </c>
       <c r="L7" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -3110,10 +3247,10 @@
         <v>97</v>
       </c>
       <c r="L8" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="9">
         <v>6</v>
       </c>
@@ -3142,10 +3279,10 @@
         <v>97</v>
       </c>
       <c r="L9" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="9">
         <v>7</v>
       </c>
@@ -3174,7 +3311,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="9">
         <v>8</v>
       </c>
@@ -3203,10 +3340,10 @@
         <v>97</v>
       </c>
       <c r="L11" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="9">
         <v>9</v>
       </c>
@@ -3235,10 +3372,10 @@
         <v>97</v>
       </c>
       <c r="L12" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="9">
         <v>10</v>
       </c>
@@ -3267,10 +3404,10 @@
         <v>96</v>
       </c>
       <c r="L13" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="9">
         <v>11</v>
       </c>
@@ -3299,10 +3436,10 @@
         <v>96</v>
       </c>
       <c r="L14" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="9">
         <v>12</v>
       </c>
@@ -3331,10 +3468,10 @@
         <v>97</v>
       </c>
       <c r="L15" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="9">
         <v>13</v>
       </c>
@@ -3363,10 +3500,10 @@
         <v>97</v>
       </c>
       <c r="L16" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="9">
         <v>14</v>
       </c>
@@ -3392,10 +3529,10 @@
         <v>97</v>
       </c>
       <c r="L17" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="9">
         <v>15</v>
       </c>
@@ -3421,7 +3558,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" s="9">
         <v>16</v>
       </c>
@@ -3447,10 +3584,10 @@
         <v>193</v>
       </c>
       <c r="L19" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="9">
         <v>17</v>
       </c>
@@ -3476,10 +3613,10 @@
         <v>194</v>
       </c>
       <c r="L20" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="9">
         <v>18</v>
       </c>
@@ -3508,10 +3645,10 @@
         <v>97</v>
       </c>
       <c r="L21" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="9">
         <v>19</v>
       </c>
@@ -3540,10 +3677,10 @@
         <v>97</v>
       </c>
       <c r="L22" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="9">
         <v>20</v>
       </c>
@@ -3572,10 +3709,10 @@
         <v>97</v>
       </c>
       <c r="L23" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="9">
         <v>21</v>
       </c>
@@ -3604,10 +3741,10 @@
         <v>96</v>
       </c>
       <c r="L24" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="9">
         <v>22</v>
       </c>
@@ -3636,10 +3773,10 @@
         <v>96</v>
       </c>
       <c r="L25" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" s="9">
         <v>23</v>
       </c>
@@ -3668,10 +3805,10 @@
         <v>97</v>
       </c>
       <c r="L26" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" s="9">
         <v>24</v>
       </c>
@@ -3700,10 +3837,10 @@
         <v>98</v>
       </c>
       <c r="L27" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" s="9">
         <v>25</v>
       </c>
@@ -3732,7 +3869,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12">
       <c r="A29" s="9">
         <v>26</v>
       </c>
@@ -3761,7 +3898,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12">
       <c r="A30" s="9">
         <v>27</v>
       </c>
@@ -3790,10 +3927,10 @@
         <v>97</v>
       </c>
       <c r="L30" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" s="9">
         <v>28</v>
       </c>
@@ -3822,10 +3959,10 @@
         <v>97</v>
       </c>
       <c r="L31" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" s="9">
         <v>29</v>
       </c>
@@ -3854,10 +3991,10 @@
         <v>97</v>
       </c>
       <c r="L32" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" s="9">
         <v>30</v>
       </c>
@@ -3886,10 +4023,10 @@
         <v>97</v>
       </c>
       <c r="L33" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" s="9">
         <v>1</v>
       </c>
@@ -3917,8 +4054,11 @@
       <c r="K36" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L36" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37" s="9">
         <v>2</v>
       </c>
@@ -3938,10 +4078,10 @@
         <v>98</v>
       </c>
       <c r="L37" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38" s="9">
         <v>3</v>
       </c>
@@ -3961,10 +4101,10 @@
         <v>98</v>
       </c>
       <c r="L38" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39" s="9">
         <v>4</v>
       </c>
@@ -3993,7 +4133,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12">
       <c r="A40" s="9">
         <v>5</v>
       </c>
@@ -4022,7 +4162,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12">
       <c r="A41" s="9">
         <v>6</v>
       </c>
@@ -4051,7 +4191,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12">
       <c r="A42" s="9">
         <v>7</v>
       </c>
@@ -4080,7 +4220,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12">
       <c r="A43" s="9">
         <v>8</v>
       </c>
@@ -4104,45 +4244,45 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B1" t="s">
         <v>259</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>260</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>261</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>262</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>263</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>264</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>265</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>266</v>
       </c>
-      <c r="K1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4171,7 +4311,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4200,7 +4340,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>1</v>
       </c>
@@ -4229,7 +4369,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>1</v>
       </c>
@@ -4258,7 +4398,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>1</v>
       </c>
@@ -4287,7 +4427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>0</v>
       </c>
@@ -4316,7 +4456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>0</v>
       </c>
@@ -4345,7 +4485,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>0</v>
       </c>
@@ -4374,7 +4514,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="F10" t="s">
         <v>93</v>
       </c>
@@ -4388,7 +4528,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>1</v>
       </c>
@@ -4417,7 +4557,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13">
         <v>1</v>
       </c>
@@ -4446,7 +4586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14">
         <v>0</v>
       </c>
@@ -4475,7 +4615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Assigned buffers and added drv8833c libs
</commit_message>
<xml_diff>
--- a/docs/TPCape_RevA_BOM.xlsx
+++ b/docs/TPCape_RevA_BOM.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\thermal-printer\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="9390" windowHeight="11655" activeTab="1"/>
   </bookViews>
@@ -12,12 +17,12 @@
     <sheet name="interface" sheetId="6" r:id="rId3"/>
     <sheet name="motor" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725" iterate="1" iterateCount="10000"/>
+  <calcPr calcId="152511" iterate="1" iterateCount="10000"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="295">
   <si>
     <t>Capture CIS Standard Bill Of Materials - Standard Report</t>
   </si>
@@ -896,17 +901,23 @@
   </si>
   <si>
     <t>head signal</t>
+  </si>
+  <si>
+    <t>Buffer output enable</t>
+  </si>
+  <si>
+    <t>LCD_AC_BIAS_EN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="g"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -950,7 +961,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -960,6 +971,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1006,7 +1035,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1029,6 +1058,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1091,7 +1129,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1123,9 +1161,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1157,6 +1196,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1332,14 +1372,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" customWidth="1"/>
     <col min="2" max="2" width="4.5703125" bestFit="1" customWidth="1"/>
@@ -1356,7 +1396,7 @@
     <col min="13" max="13" width="62.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1366,7 +1406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1377,27 +1417,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1438,7 +1478,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -1465,7 +1505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -1492,7 +1532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>3</v>
       </c>
@@ -1531,7 +1571,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>4</v>
       </c>
@@ -1570,7 +1610,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>5</v>
       </c>
@@ -1599,7 +1639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>6</v>
       </c>
@@ -1639,7 +1679,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>7</v>
       </c>
@@ -1657,7 +1697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>8</v>
       </c>
@@ -1675,7 +1715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>9</v>
       </c>
@@ -1693,7 +1733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>10</v>
       </c>
@@ -1702,7 +1742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>11</v>
       </c>
@@ -1732,7 +1772,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>12</v>
       </c>
@@ -1741,7 +1781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>13</v>
       </c>
@@ -1750,7 +1790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>14</v>
       </c>
@@ -1759,7 +1799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>15</v>
       </c>
@@ -1768,7 +1808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>16</v>
       </c>
@@ -1777,7 +1817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>17</v>
       </c>
@@ -1792,7 +1832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>18</v>
       </c>
@@ -1816,7 +1856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>19</v>
       </c>
@@ -1840,7 +1880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>20</v>
       </c>
@@ -1864,7 +1904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>21</v>
       </c>
@@ -1888,7 +1928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>22</v>
       </c>
@@ -1897,7 +1937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>23</v>
       </c>
@@ -1906,7 +1946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>24</v>
       </c>
@@ -1930,7 +1970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>25</v>
       </c>
@@ -1947,7 +1987,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>26</v>
       </c>
@@ -1964,7 +2004,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>27</v>
       </c>
@@ -1984,7 +2024,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>28</v>
       </c>
@@ -2001,7 +2041,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>29</v>
       </c>
@@ -2018,12 +2058,12 @@
         <v>234</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>31</v>
       </c>
@@ -2034,22 +2074,22 @@
         <v>241</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>25</v>
       </c>
@@ -2100,14 +2140,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" customWidth="1"/>
     <col min="3" max="3" width="3.85546875" bestFit="1" customWidth="1"/>
@@ -2116,12 +2156,12 @@
     <col min="7" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -2141,7 +2181,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -2164,7 +2204,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -2187,7 +2227,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -2206,7 +2246,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -2225,8 +2265,17 @@
       <c r="F7" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="G7" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="H7" t="s">
+        <v>138</v>
+      </c>
+      <c r="I7" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -2245,37 +2294,66 @@
       <c r="F8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="G8" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="H8" t="s">
+        <v>158</v>
+      </c>
+      <c r="I8" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>6</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="15" t="s">
         <v>78</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="9"/>
+      <c r="D9" t="s">
+        <v>172</v>
+      </c>
+      <c r="E9" t="s">
+        <v>132</v>
+      </c>
       <c r="F9" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="G9" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="H9" t="s">
+        <v>147</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>7</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="15" t="s">
         <v>79</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>97</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="E10" t="s">
+        <v>137</v>
       </c>
       <c r="F10" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>8</v>
       </c>
@@ -2295,7 +2373,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>9</v>
       </c>
@@ -2315,97 +2393,94 @@
         <v>105</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
       <c r="H12" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>148</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>10</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="16" t="s">
         <v>81</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D13" s="9" t="s">
-        <v>166</v>
+      <c r="D13" t="s">
+        <v>171</v>
       </c>
       <c r="E13" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="F13" t="s">
         <v>106</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="H13" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>11</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="16" t="s">
         <v>82</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>165</v>
+      <c r="D14" t="s">
+        <v>170</v>
       </c>
       <c r="E14" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="F14" t="s">
         <v>107</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="H14" t="s">
-        <v>148</v>
-      </c>
-      <c r="I14" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>12</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="16" t="s">
         <v>83</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>164</v>
+      <c r="D15" t="s">
+        <v>153</v>
       </c>
       <c r="E15" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="F15" t="s">
         <v>108</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="H15" t="s">
-        <v>149</v>
-      </c>
-      <c r="I15" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>13</v>
       </c>
@@ -2424,14 +2499,8 @@
       <c r="F16" t="s">
         <v>112</v>
       </c>
-      <c r="G16" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="H16" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>14</v>
       </c>
@@ -2446,14 +2515,8 @@
       <c r="F17" t="s">
         <v>113</v>
       </c>
-      <c r="G17" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="H17" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>15</v>
       </c>
@@ -2468,92 +2531,68 @@
       <c r="F18" t="s">
         <v>113</v>
       </c>
-      <c r="G18" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="H18" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>16</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="16" t="s">
         <v>86</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>156</v>
+      <c r="D19" t="s">
+        <v>152</v>
       </c>
       <c r="E19" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="F19" t="s">
         <v>109</v>
       </c>
-      <c r="G19" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="H19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>17</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="16" t="s">
         <v>87</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>157</v>
+      <c r="D20" t="s">
+        <v>151</v>
       </c>
       <c r="E20" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F20" t="s">
         <v>110</v>
       </c>
-      <c r="G20" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="H20" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>18</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="16" t="s">
         <v>88</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D21" s="9" t="s">
-        <v>155</v>
+      <c r="D21" t="s">
+        <v>150</v>
       </c>
       <c r="E21" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F21" t="s">
         <v>111</v>
       </c>
-      <c r="G21" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="H21" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>19</v>
       </c>
@@ -2573,7 +2612,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>20</v>
       </c>
@@ -2593,41 +2632,47 @@
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>21</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="15" t="s">
         <v>89</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>97</v>
+      </c>
+      <c r="D24" t="s">
+        <v>173</v>
+      </c>
+      <c r="E24" t="s">
+        <v>129</v>
       </c>
       <c r="F24" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>22</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="14" t="s">
         <v>90</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>98</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="E25" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="F25" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>23</v>
       </c>
@@ -2647,7 +2692,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>24</v>
       </c>
@@ -2667,7 +2712,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>25</v>
       </c>
@@ -2685,7 +2730,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>26</v>
       </c>
@@ -2701,87 +2746,87 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>27</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="15" t="s">
         <v>92</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D30" t="s">
-        <v>151</v>
+      <c r="D30" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="E30" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F30" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>28</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="15" t="s">
         <v>93</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D31" t="s">
-        <v>150</v>
+      <c r="D31" s="9" t="s">
+        <v>154</v>
       </c>
       <c r="E31" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="F31" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>29</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="15" t="s">
         <v>94</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D32" t="s">
-        <v>153</v>
+      <c r="D32" s="9" t="s">
+        <v>157</v>
       </c>
       <c r="E32" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="F32" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
         <v>30</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="15" t="s">
         <v>95</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D33" t="s">
-        <v>152</v>
+      <c r="D33" s="9" t="s">
+        <v>156</v>
       </c>
       <c r="E33" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="F33" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <v>1</v>
       </c>
@@ -2804,7 +2849,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>2</v>
       </c>
@@ -2821,7 +2866,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <v>3</v>
       </c>
@@ -2844,87 +2889,87 @@
         <v>183</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <v>4</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="15" t="s">
         <v>93</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D39" t="s">
-        <v>170</v>
+      <c r="D39" s="9" t="s">
+        <v>164</v>
       </c>
       <c r="E39" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="F39" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <v>5</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="15" t="s">
         <v>92</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D40" t="s">
-        <v>171</v>
+      <c r="D40" s="9" t="s">
+        <v>165</v>
       </c>
       <c r="E40" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="F40" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
         <v>6</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="15" t="s">
         <v>95</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D41" t="s">
-        <v>172</v>
+      <c r="D41" s="9" t="s">
+        <v>166</v>
       </c>
       <c r="E41" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="F41" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>7</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="15" t="s">
         <v>94</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D42" t="s">
-        <v>173</v>
+      <c r="D42" s="9" t="s">
+        <v>167</v>
       </c>
       <c r="E42" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="F42" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
         <v>8</v>
       </c>
@@ -2935,7 +2980,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>6</v>
       </c>
@@ -2946,7 +2991,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>3</v>
       </c>
@@ -2957,7 +3002,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>4</v>
       </c>
@@ -2968,7 +3013,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>4</v>
       </c>
@@ -2979,7 +3024,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1</v>
       </c>
@@ -2990,7 +3035,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2</v>
       </c>
@@ -3001,7 +3046,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2</v>
       </c>
@@ -3012,7 +3057,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1</v>
       </c>
@@ -3023,7 +3068,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <f>SUM(A47:A52)</f>
         <v>20</v>
@@ -3035,24 +3080,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M43"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="12" max="12" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -3084,7 +3129,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -3116,7 +3161,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -3151,7 +3196,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -3186,7 +3231,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -3218,7 +3263,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -3250,7 +3295,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>6</v>
       </c>
@@ -3282,7 +3327,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>7</v>
       </c>
@@ -3311,7 +3356,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>8</v>
       </c>
@@ -3343,7 +3388,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>9</v>
       </c>
@@ -3375,7 +3420,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>10</v>
       </c>
@@ -3407,7 +3452,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>11</v>
       </c>
@@ -3439,7 +3484,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>12</v>
       </c>
@@ -3471,7 +3516,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>13</v>
       </c>
@@ -3503,7 +3548,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>14</v>
       </c>
@@ -3532,7 +3577,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>15</v>
       </c>
@@ -3558,7 +3603,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>16</v>
       </c>
@@ -3587,7 +3632,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>17</v>
       </c>
@@ -3616,7 +3661,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>18</v>
       </c>
@@ -3648,7 +3693,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>19</v>
       </c>
@@ -3680,7 +3725,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>20</v>
       </c>
@@ -3712,7 +3757,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>21</v>
       </c>
@@ -3744,7 +3789,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>22</v>
       </c>
@@ -3776,7 +3821,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>23</v>
       </c>
@@ -3808,7 +3853,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>24</v>
       </c>
@@ -3840,7 +3885,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>25</v>
       </c>
@@ -3869,7 +3914,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>26</v>
       </c>
@@ -3898,7 +3943,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>27</v>
       </c>
@@ -3930,7 +3975,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>28</v>
       </c>
@@ -3962,7 +4007,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>29</v>
       </c>
@@ -3994,7 +4039,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
         <v>30</v>
       </c>
@@ -4026,7 +4071,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <v>1</v>
       </c>
@@ -4058,7 +4103,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>2</v>
       </c>
@@ -4081,7 +4126,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <v>3</v>
       </c>
@@ -4104,7 +4149,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <v>4</v>
       </c>
@@ -4133,7 +4178,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <v>5</v>
       </c>
@@ -4162,7 +4207,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
         <v>6</v>
       </c>
@@ -4191,7 +4236,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>7</v>
       </c>
@@ -4220,7 +4265,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
         <v>8</v>
       </c>
@@ -4244,16 +4289,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>258</v>
       </c>
@@ -4282,7 +4327,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4311,7 +4356,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4340,7 +4385,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -4369,7 +4414,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -4398,7 +4443,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -4427,7 +4472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -4456,7 +4501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -4485,7 +4530,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -4514,7 +4559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
         <v>93</v>
       </c>
@@ -4528,7 +4573,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -4557,7 +4602,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -4586,7 +4631,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -4615,7 +4660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Added external pulls and decaps
</commit_message>
<xml_diff>
--- a/docs/TPCape_RevA_BOM.xlsx
+++ b/docs/TPCape_RevA_BOM.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\thermal-printer\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="9390" windowHeight="11655" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="9390" windowHeight="11655" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TPcape_BOM" sheetId="4" r:id="rId1"/>
@@ -17,12 +12,12 @@
     <sheet name="interface" sheetId="6" r:id="rId3"/>
     <sheet name="motor" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511" iterate="1" iterateCount="10000"/>
+  <calcPr calcId="125725" iterate="1" iterateCount="10000"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="298">
   <si>
     <t>Capture CIS Standard Bill Of Materials - Standard Report</t>
   </si>
@@ -786,9 +781,6 @@
     <t>R33, R63</t>
   </si>
   <si>
-    <t xml:space="preserve">0603 x 4, </t>
-  </si>
-  <si>
     <t xml:space="preserve">0402, 5%, </t>
   </si>
   <si>
@@ -907,17 +899,29 @@
   </si>
   <si>
     <t>LCD_AC_BIAS_EN</t>
+  </si>
+  <si>
+    <t>RES ARRAY 22K OHM 4 RES 1206</t>
+  </si>
+  <si>
+    <t>22K</t>
+  </si>
+  <si>
+    <t>1000pF</t>
+  </si>
+  <si>
+    <t>CAP ARRAY 1000PF 100V X7R 1206</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="g"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1129,7 +1133,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1161,10 +1165,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1196,7 +1199,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1372,14 +1374,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.42578125" customWidth="1"/>
     <col min="2" max="2" width="4.5703125" bestFit="1" customWidth="1"/>
@@ -1396,7 +1398,7 @@
     <col min="13" max="13" width="62.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1406,7 +1408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1417,27 +1419,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1478,7 +1480,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -1505,7 +1507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -1532,7 +1534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="1">
         <v>3</v>
       </c>
@@ -1571,7 +1573,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="1">
         <v>4</v>
       </c>
@@ -1610,7 +1612,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" s="1">
         <v>5</v>
       </c>
@@ -1639,7 +1641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" s="1">
         <v>6</v>
       </c>
@@ -1679,7 +1681,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" s="1">
         <v>7</v>
       </c>
@@ -1697,7 +1699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" s="1">
         <v>8</v>
       </c>
@@ -1715,7 +1717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="A17" s="1">
         <v>9</v>
       </c>
@@ -1733,7 +1735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" s="1">
         <v>10</v>
       </c>
@@ -1742,7 +1744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" s="1">
         <v>11</v>
       </c>
@@ -1750,19 +1752,19 @@
         <v>1</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I19" t="s">
         <v>35</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K19" s="6">
         <v>0.73</v>
@@ -1772,7 +1774,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" s="1">
         <v>12</v>
       </c>
@@ -1781,7 +1783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21" s="1">
         <v>13</v>
       </c>
@@ -1790,7 +1792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" s="1">
         <v>14</v>
       </c>
@@ -1799,7 +1801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23" s="1">
         <v>15</v>
       </c>
@@ -1808,7 +1810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="A24" s="1">
         <v>16</v>
       </c>
@@ -1817,13 +1819,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12">
       <c r="A25" s="1">
         <v>17</v>
       </c>
       <c r="C25" t="s">
         <v>235</v>
       </c>
+      <c r="D25" t="s">
+        <v>296</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>297</v>
+      </c>
       <c r="G25" s="2" t="s">
         <v>233</v>
       </c>
@@ -1832,31 +1840,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26" s="1">
         <v>18</v>
       </c>
       <c r="C26" t="s">
+        <v>273</v>
+      </c>
+      <c r="D26" t="s">
+        <v>278</v>
+      </c>
+      <c r="E26" t="s">
+        <v>279</v>
+      </c>
+      <c r="F26" t="s">
+        <v>275</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>274</v>
-      </c>
-      <c r="D26" t="s">
-        <v>279</v>
-      </c>
-      <c r="E26" t="s">
-        <v>280</v>
-      </c>
-      <c r="F26" t="s">
-        <v>276</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>275</v>
       </c>
       <c r="L26" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="A27" s="1">
         <v>19</v>
       </c>
@@ -1880,7 +1888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12">
       <c r="A28" s="1">
         <v>20</v>
       </c>
@@ -1904,7 +1912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12">
       <c r="A29" s="1">
         <v>21</v>
       </c>
@@ -1928,7 +1936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12">
       <c r="A30" s="1">
         <v>22</v>
       </c>
@@ -1937,7 +1945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12">
       <c r="A31" s="1">
         <v>23</v>
       </c>
@@ -1946,7 +1954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12">
       <c r="A32" s="1">
         <v>24</v>
       </c>
@@ -1970,7 +1978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12">
       <c r="A33" s="1">
         <v>25</v>
       </c>
@@ -1978,7 +1986,7 @@
         <v>230</v>
       </c>
       <c r="E33" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F33" t="s">
         <v>244</v>
@@ -1987,7 +1995,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12">
       <c r="A34" s="1">
         <v>26</v>
       </c>
@@ -1995,7 +2003,7 @@
         <v>232</v>
       </c>
       <c r="E34" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F34" t="s">
         <v>244</v>
@@ -2004,7 +2012,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12">
       <c r="A35" s="1">
         <v>27</v>
       </c>
@@ -2024,7 +2032,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12">
       <c r="A36" s="1">
         <v>28</v>
       </c>
@@ -2032,7 +2040,7 @@
         <v>243</v>
       </c>
       <c r="E36" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F36" t="s">
         <v>244</v>
@@ -2041,15 +2049,18 @@
         <v>205</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12">
       <c r="A37" s="1">
         <v>29</v>
       </c>
       <c r="C37" t="s">
         <v>240</v>
       </c>
-      <c r="E37" t="s">
-        <v>254</v>
+      <c r="D37" t="s">
+        <v>295</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>294</v>
       </c>
       <c r="F37" t="s">
         <v>244</v>
@@ -2058,12 +2069,12 @@
         <v>234</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12">
       <c r="A38" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12">
       <c r="A39" s="1">
         <v>31</v>
       </c>
@@ -2074,22 +2085,22 @@
         <v>241</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12">
       <c r="A40" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12">
       <c r="A41" s="1">
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12">
       <c r="A42" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12">
       <c r="A43" s="1">
         <v>25</v>
       </c>
@@ -2140,28 +2151,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.140625" customWidth="1"/>
     <col min="3" max="3" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="45.7109375" customWidth="1"/>
-    <col min="7" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -2181,7 +2192,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -2200,11 +2211,11 @@
       <c r="F4" t="s">
         <v>99</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="H4" s="10" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -2223,11 +2234,11 @@
       <c r="F5" t="s">
         <v>100</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="H5" s="10" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -2242,11 +2253,11 @@
       <c r="F6" t="s">
         <v>101</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="H6" s="10" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -2265,17 +2276,17 @@
       <c r="F7" t="s">
         <v>102</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="H7" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>138</v>
       </c>
-      <c r="I7" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -2294,17 +2305,17 @@
       <c r="F8" t="s">
         <v>102</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="H8" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>158</v>
       </c>
-      <c r="I8" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="9">
         <v>6</v>
       </c>
@@ -2323,17 +2334,17 @@
       <c r="F9" t="s">
         <v>103</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="H9" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>147</v>
       </c>
-      <c r="I9" s="10" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="10" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="9">
         <v>7</v>
       </c>
@@ -2353,7 +2364,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="9">
         <v>8</v>
       </c>
@@ -2373,7 +2384,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="9">
         <v>9</v>
       </c>
@@ -2392,17 +2403,17 @@
       <c r="F12" t="s">
         <v>105</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="H12" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>148</v>
       </c>
-      <c r="I12" s="10" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="9">
         <v>10</v>
       </c>
@@ -2421,14 +2432,14 @@
       <c r="F13" t="s">
         <v>106</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="H13" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="9">
         <v>11</v>
       </c>
@@ -2447,14 +2458,14 @@
       <c r="F14" t="s">
         <v>107</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="H14" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="9">
         <v>12</v>
       </c>
@@ -2473,14 +2484,14 @@
       <c r="F15" t="s">
         <v>108</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="H15" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="9">
         <v>13</v>
       </c>
@@ -2500,7 +2511,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="9">
         <v>14</v>
       </c>
@@ -2516,7 +2527,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="9">
         <v>15</v>
       </c>
@@ -2532,7 +2543,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="9">
         <v>16</v>
       </c>
@@ -2552,7 +2563,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="9">
         <v>17</v>
       </c>
@@ -2572,7 +2583,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="9">
         <v>18</v>
       </c>
@@ -2592,7 +2603,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="9">
         <v>19</v>
       </c>
@@ -2612,7 +2623,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="9">
         <v>20</v>
       </c>
@@ -2632,7 +2643,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="9">
         <v>21</v>
       </c>
@@ -2652,7 +2663,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="9">
         <v>22</v>
       </c>
@@ -2672,7 +2683,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="9">
         <v>23</v>
       </c>
@@ -2692,7 +2703,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="9">
         <v>24</v>
       </c>
@@ -2712,7 +2723,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="9">
         <v>25</v>
       </c>
@@ -2730,7 +2741,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="9">
         <v>26</v>
       </c>
@@ -2746,7 +2757,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="9">
         <v>27</v>
       </c>
@@ -2766,7 +2777,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="9">
         <v>28</v>
       </c>
@@ -2786,7 +2797,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="9">
         <v>29</v>
       </c>
@@ -2806,7 +2817,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="9">
         <v>30</v>
       </c>
@@ -2826,7 +2837,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="9">
         <v>1</v>
       </c>
@@ -2845,11 +2856,11 @@
       <c r="F36" t="s">
         <v>122</v>
       </c>
-      <c r="G36" s="10" t="s">
+      <c r="H36" s="10" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="9">
         <v>2</v>
       </c>
@@ -2862,11 +2873,11 @@
       <c r="F37" t="s">
         <v>101</v>
       </c>
-      <c r="G37" s="10" t="s">
+      <c r="H37" s="10" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="9">
         <v>3</v>
       </c>
@@ -2885,11 +2896,11 @@
       <c r="F38" t="s">
         <v>99</v>
       </c>
-      <c r="G38" s="10" t="s">
+      <c r="H38" s="10" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="9">
         <v>4</v>
       </c>
@@ -2909,7 +2920,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="9">
         <v>5</v>
       </c>
@@ -2929,7 +2940,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="9">
         <v>6</v>
       </c>
@@ -2949,7 +2960,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="9">
         <v>7</v>
       </c>
@@ -2969,7 +2980,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" s="9">
         <v>8</v>
       </c>
@@ -2980,95 +2991,95 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47">
         <v>6</v>
       </c>
       <c r="B47" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E47" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48">
         <v>3</v>
       </c>
       <c r="B48" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E48" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49">
         <v>4</v>
       </c>
       <c r="B49" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E49" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50">
         <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E50" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51">
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E51" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52">
         <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E52" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53">
         <v>2</v>
       </c>
       <c r="B53" t="s">
+        <v>270</v>
+      </c>
+      <c r="E53" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54" t="s">
         <v>271</v>
       </c>
-      <c r="E53" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>1</v>
-      </c>
-      <c r="B54" t="s">
-        <v>272</v>
-      </c>
       <c r="E54" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56">
         <f>SUM(A47:A52)</f>
         <v>20</v>
@@ -3080,24 +3091,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:M43"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="12" max="12" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="B2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -3129,7 +3140,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -3161,7 +3172,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -3193,10 +3204,10 @@
         <v>207</v>
       </c>
       <c r="M5" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -3228,10 +3239,10 @@
         <v>206</v>
       </c>
       <c r="M6" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -3263,7 +3274,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -3292,10 +3303,10 @@
         <v>97</v>
       </c>
       <c r="L8" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="9">
         <v>6</v>
       </c>
@@ -3327,7 +3338,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" s="9">
         <v>7</v>
       </c>
@@ -3356,7 +3367,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="9">
         <v>8</v>
       </c>
@@ -3388,7 +3399,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="9">
         <v>9</v>
       </c>
@@ -3420,7 +3431,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" s="9">
         <v>10</v>
       </c>
@@ -3452,7 +3463,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" s="9">
         <v>11</v>
       </c>
@@ -3484,7 +3495,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" s="9">
         <v>12</v>
       </c>
@@ -3516,7 +3527,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" s="9">
         <v>13</v>
       </c>
@@ -3545,10 +3556,10 @@
         <v>97</v>
       </c>
       <c r="L16" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="9">
         <v>14</v>
       </c>
@@ -3577,7 +3588,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" s="9">
         <v>15</v>
       </c>
@@ -3603,7 +3614,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" s="9">
         <v>16</v>
       </c>
@@ -3632,7 +3643,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" s="9">
         <v>17</v>
       </c>
@@ -3661,7 +3672,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21" s="9">
         <v>18</v>
       </c>
@@ -3693,7 +3704,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" s="9">
         <v>19</v>
       </c>
@@ -3725,7 +3736,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23" s="9">
         <v>20</v>
       </c>
@@ -3757,7 +3768,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="A24" s="9">
         <v>21</v>
       </c>
@@ -3789,7 +3800,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12">
       <c r="A25" s="9">
         <v>22</v>
       </c>
@@ -3821,7 +3832,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26" s="9">
         <v>23</v>
       </c>
@@ -3853,7 +3864,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="A27" s="9">
         <v>24</v>
       </c>
@@ -3885,7 +3896,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12">
       <c r="A28" s="9">
         <v>25</v>
       </c>
@@ -3914,7 +3925,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12">
       <c r="A29" s="9">
         <v>26</v>
       </c>
@@ -3943,7 +3954,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12">
       <c r="A30" s="9">
         <v>27</v>
       </c>
@@ -3975,7 +3986,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12">
       <c r="A31" s="9">
         <v>28</v>
       </c>
@@ -4007,7 +4018,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12">
       <c r="A32" s="9">
         <v>29</v>
       </c>
@@ -4039,7 +4050,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12">
       <c r="A33" s="9">
         <v>30</v>
       </c>
@@ -4071,7 +4082,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12">
       <c r="A36" s="9">
         <v>1</v>
       </c>
@@ -4100,10 +4111,10 @@
         <v>97</v>
       </c>
       <c r="L36" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37" s="9">
         <v>2</v>
       </c>
@@ -4126,7 +4137,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12">
       <c r="A38" s="9">
         <v>3</v>
       </c>
@@ -4149,7 +4160,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12">
       <c r="A39" s="9">
         <v>4</v>
       </c>
@@ -4178,7 +4189,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12">
       <c r="A40" s="9">
         <v>5</v>
       </c>
@@ -4207,7 +4218,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12">
       <c r="A41" s="9">
         <v>6</v>
       </c>
@@ -4236,7 +4247,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12">
       <c r="A42" s="9">
         <v>7</v>
       </c>
@@ -4265,7 +4276,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12">
       <c r="A43" s="9">
         <v>8</v>
       </c>
@@ -4289,45 +4300,45 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" t="s">
         <v>258</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>259</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>260</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>261</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>262</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>263</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>264</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>265</v>
       </c>
-      <c r="K1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4356,7 +4367,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4385,7 +4396,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>1</v>
       </c>
@@ -4414,7 +4425,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>1</v>
       </c>
@@ -4443,7 +4454,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>1</v>
       </c>
@@ -4472,7 +4483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>0</v>
       </c>
@@ -4501,7 +4512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>0</v>
       </c>
@@ -4530,7 +4541,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>0</v>
       </c>
@@ -4559,7 +4570,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="F10" t="s">
         <v>93</v>
       </c>
@@ -4573,7 +4584,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>1</v>
       </c>
@@ -4602,7 +4613,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13">
         <v>1</v>
       </c>
@@ -4631,7 +4642,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14">
         <v>0</v>
       </c>
@@ -4660,7 +4671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Added photo transistor comparator circuit
</commit_message>
<xml_diff>
--- a/docs/TPCape_RevA_BOM.xlsx
+++ b/docs/TPCape_RevA_BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="9390" windowHeight="11655" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="9390" windowHeight="11655"/>
   </bookViews>
   <sheets>
     <sheet name="TPcape_BOM" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="304">
   <si>
     <t>Capture CIS Standard Bill Of Materials - Standard Report</t>
   </si>
@@ -598,9 +598,6 @@
     <t>HCLK</t>
   </si>
   <si>
-    <t>Vref</t>
-  </si>
-  <si>
     <t>TMR2</t>
   </si>
   <si>
@@ -748,9 +745,6 @@
     <t>Q7</t>
   </si>
   <si>
-    <t>R64</t>
-  </si>
-  <si>
     <t>Rohm</t>
   </si>
   <si>
@@ -911,6 +905,30 @@
   </si>
   <si>
     <t>CAP ARRAY 1000PF 100V X7R 1206</t>
+  </si>
+  <si>
+    <t>R35, R64</t>
+  </si>
+  <si>
+    <t>R32 (), CA2 ()</t>
+  </si>
+  <si>
+    <t>4.7K</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>TMP</t>
+  </si>
+  <si>
+    <t>I?</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>MCR10HJ120</t>
   </si>
 </sst>
 </file>
@@ -1377,8 +1395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1752,19 +1770,19 @@
         <v>1</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="I19" t="s">
         <v>35</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="K19" s="6">
         <v>0.73</v>
@@ -1824,16 +1842,16 @@
         <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D25" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L25" s="6">
         <f t="shared" si="0"/>
@@ -1845,19 +1863,19 @@
         <v>18</v>
       </c>
       <c r="C26" t="s">
+        <v>271</v>
+      </c>
+      <c r="D26" t="s">
+        <v>276</v>
+      </c>
+      <c r="E26" t="s">
+        <v>277</v>
+      </c>
+      <c r="F26" t="s">
         <v>273</v>
       </c>
-      <c r="D26" t="s">
-        <v>278</v>
-      </c>
-      <c r="E26" t="s">
-        <v>279</v>
-      </c>
-      <c r="F26" t="s">
-        <v>275</v>
-      </c>
       <c r="G26" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L26" s="6">
         <f t="shared" si="0"/>
@@ -1869,19 +1887,19 @@
         <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D27" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E27" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F27" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L27" s="6">
         <f t="shared" si="0"/>
@@ -1893,19 +1911,19 @@
         <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D28" t="s">
+        <v>222</v>
+      </c>
+      <c r="E28" t="s">
         <v>223</v>
       </c>
-      <c r="E28" t="s">
-        <v>224</v>
-      </c>
       <c r="F28" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L28" s="6">
         <f t="shared" si="0"/>
@@ -1917,19 +1935,19 @@
         <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D29" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E29" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F29" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L29" s="6">
         <f t="shared" si="0"/>
@@ -1949,6 +1967,21 @@
       <c r="A31" s="1">
         <v>23</v>
       </c>
+      <c r="C31" t="s">
+        <v>302</v>
+      </c>
+      <c r="D31">
+        <v>12</v>
+      </c>
+      <c r="E31" t="s">
+        <v>254</v>
+      </c>
+      <c r="F31" t="s">
+        <v>242</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>303</v>
+      </c>
       <c r="L31" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1959,19 +1992,19 @@
         <v>24</v>
       </c>
       <c r="C32" t="s">
+        <v>236</v>
+      </c>
+      <c r="D32" t="s">
+        <v>250</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="F32" t="s">
+        <v>242</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="D32" t="s">
-        <v>252</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>251</v>
-      </c>
-      <c r="F32" t="s">
-        <v>244</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>238</v>
       </c>
       <c r="L32" s="6">
         <f t="shared" si="0"/>
@@ -1983,16 +2016,19 @@
         <v>25</v>
       </c>
       <c r="C33" t="s">
-        <v>230</v>
+        <v>229</v>
+      </c>
+      <c r="D33" t="s">
+        <v>299</v>
       </c>
       <c r="E33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F33" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -2000,16 +2036,19 @@
         <v>26</v>
       </c>
       <c r="C34" t="s">
-        <v>232</v>
+        <v>231</v>
+      </c>
+      <c r="D34" t="s">
+        <v>298</v>
       </c>
       <c r="E34" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F34" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -2017,19 +2056,19 @@
         <v>27</v>
       </c>
       <c r="C35" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D35" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E35" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F35" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -2037,16 +2076,19 @@
         <v>28</v>
       </c>
       <c r="C36" t="s">
-        <v>243</v>
+        <v>296</v>
+      </c>
+      <c r="D36">
+        <v>180</v>
       </c>
       <c r="E36" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F36" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -2054,19 +2096,19 @@
         <v>29</v>
       </c>
       <c r="C37" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D37" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F37" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -2079,10 +2121,10 @@
         <v>31</v>
       </c>
       <c r="C39" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -2154,7 +2196,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
@@ -2235,7 +2277,7 @@
         <v>100</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -2283,7 +2325,7 @@
         <v>138</v>
       </c>
       <c r="J7" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -2312,7 +2354,7 @@
         <v>158</v>
       </c>
       <c r="J8" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2341,7 +2383,7 @@
         <v>147</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -2410,7 +2452,7 @@
         <v>148</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -2857,7 +2899,7 @@
         <v>122</v>
       </c>
       <c r="H36" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -2996,10 +3038,10 @@
         <v>6</v>
       </c>
       <c r="B47" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E47" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -3007,10 +3049,10 @@
         <v>3</v>
       </c>
       <c r="B48" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E48" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -3018,10 +3060,10 @@
         <v>4</v>
       </c>
       <c r="B49" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E49" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -3029,10 +3071,10 @@
         <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E50" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -3040,10 +3082,10 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E51" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -3051,10 +3093,10 @@
         <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E52" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -3062,10 +3104,10 @@
         <v>2</v>
       </c>
       <c r="B53" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E53" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -3073,10 +3115,10 @@
         <v>1</v>
       </c>
       <c r="B54" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E54" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -3094,8 +3136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3154,7 +3196,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G4" t="s">
         <v>96</v>
@@ -3163,13 +3205,13 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K4" t="s">
         <v>96</v>
       </c>
       <c r="L4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -3201,10 +3243,10 @@
         <v>97</v>
       </c>
       <c r="L5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -3236,10 +3278,10 @@
         <v>98</v>
       </c>
       <c r="L6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M6" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -3271,7 +3313,7 @@
         <v>98</v>
       </c>
       <c r="L7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -3303,7 +3345,7 @@
         <v>97</v>
       </c>
       <c r="L8" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -3335,7 +3377,7 @@
         <v>97</v>
       </c>
       <c r="L9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -3396,7 +3438,7 @@
         <v>97</v>
       </c>
       <c r="L11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -3428,7 +3470,7 @@
         <v>97</v>
       </c>
       <c r="L12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -3460,7 +3502,7 @@
         <v>96</v>
       </c>
       <c r="L13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -3492,7 +3534,7 @@
         <v>96</v>
       </c>
       <c r="L14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -3524,7 +3566,7 @@
         <v>97</v>
       </c>
       <c r="L15" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -3556,7 +3598,7 @@
         <v>97</v>
       </c>
       <c r="L16" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -3573,7 +3615,10 @@
         <v>16</v>
       </c>
       <c r="F17" t="s">
-        <v>193</v>
+        <v>300</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>98</v>
       </c>
       <c r="I17" s="9">
         <v>14</v>
@@ -3585,7 +3630,7 @@
         <v>97</v>
       </c>
       <c r="L17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -3602,7 +3647,10 @@
         <v>17</v>
       </c>
       <c r="F18" t="s">
-        <v>194</v>
+        <v>193</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>301</v>
       </c>
       <c r="I18" s="9">
         <v>15</v>
@@ -3637,10 +3685,13 @@
         <v>16</v>
       </c>
       <c r="J19" t="s">
-        <v>193</v>
+        <v>300</v>
+      </c>
+      <c r="K19" t="s">
+        <v>98</v>
       </c>
       <c r="L19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -3666,10 +3717,13 @@
         <v>17</v>
       </c>
       <c r="J20" t="s">
-        <v>194</v>
+        <v>193</v>
+      </c>
+      <c r="K20" t="s">
+        <v>301</v>
       </c>
       <c r="L20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -3701,7 +3755,7 @@
         <v>97</v>
       </c>
       <c r="L21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -3733,7 +3787,7 @@
         <v>97</v>
       </c>
       <c r="L22" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -3765,7 +3819,7 @@
         <v>97</v>
       </c>
       <c r="L23" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -3782,7 +3836,7 @@
         <v>23</v>
       </c>
       <c r="F24" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G24" t="s">
         <v>97</v>
@@ -3797,7 +3851,7 @@
         <v>96</v>
       </c>
       <c r="L24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -3829,7 +3883,7 @@
         <v>96</v>
       </c>
       <c r="L25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -3855,13 +3909,13 @@
         <v>23</v>
       </c>
       <c r="J26" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K26" t="s">
         <v>97</v>
       </c>
       <c r="L26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -3893,7 +3947,7 @@
         <v>98</v>
       </c>
       <c r="L27" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -3953,6 +4007,9 @@
       <c r="K29" t="s">
         <v>97</v>
       </c>
+      <c r="L29" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="9">
@@ -3983,7 +4040,7 @@
         <v>97</v>
       </c>
       <c r="L30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -4015,7 +4072,7 @@
         <v>97</v>
       </c>
       <c r="L31" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -4047,7 +4104,7 @@
         <v>97</v>
       </c>
       <c r="L32" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -4079,7 +4136,7 @@
         <v>97</v>
       </c>
       <c r="L33" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -4111,7 +4168,7 @@
         <v>97</v>
       </c>
       <c r="L36" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -4128,13 +4185,13 @@
         <v>2</v>
       </c>
       <c r="J37" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K37" t="s">
         <v>98</v>
       </c>
       <c r="L37" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -4151,13 +4208,13 @@
         <v>3</v>
       </c>
       <c r="J38" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K38" t="s">
         <v>98</v>
       </c>
       <c r="L38" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -4174,7 +4231,7 @@
         <v>4</v>
       </c>
       <c r="F39" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G39" t="s">
         <v>97</v>
@@ -4183,7 +4240,7 @@
         <v>4</v>
       </c>
       <c r="J39" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K39" t="s">
         <v>97</v>
@@ -4203,7 +4260,7 @@
         <v>5</v>
       </c>
       <c r="F40" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G40" t="s">
         <v>97</v>
@@ -4212,7 +4269,7 @@
         <v>5</v>
       </c>
       <c r="J40" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K40" t="s">
         <v>97</v>
@@ -4232,7 +4289,7 @@
         <v>6</v>
       </c>
       <c r="F41" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G41" t="s">
         <v>97</v>
@@ -4241,7 +4298,7 @@
         <v>6</v>
       </c>
       <c r="J41" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K41" t="s">
         <v>97</v>
@@ -4261,7 +4318,7 @@
         <v>7</v>
       </c>
       <c r="F42" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G42" t="s">
         <v>97</v>
@@ -4270,7 +4327,7 @@
         <v>7</v>
       </c>
       <c r="J42" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K42" t="s">
         <v>97</v>
@@ -4311,31 +4368,31 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C1" t="s">
         <v>257</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>258</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>259</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>260</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>261</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>262</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>263</v>
-      </c>
-      <c r="I1" t="s">
-        <v>264</v>
-      </c>
-      <c r="K1" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:11">

</xml_diff>

<commit_message>
Added power circuit, cleaned up comparator docs
</commit_message>
<xml_diff>
--- a/docs/TPCape_RevA_BOM.xlsx
+++ b/docs/TPCape_RevA_BOM.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\thermal-printer\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="9390" windowHeight="11655"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="5970" windowHeight="5670" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TPcape_BOM" sheetId="4" r:id="rId1"/>
@@ -12,12 +17,12 @@
     <sheet name="interface" sheetId="6" r:id="rId3"/>
     <sheet name="motor" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725" iterate="1" iterateCount="10000"/>
+  <calcPr calcId="152511" iterate="1" iterateCount="10000"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="312">
   <si>
     <t>Capture CIS Standard Bill Of Materials - Standard Report</t>
   </si>
@@ -929,17 +934,41 @@
   </si>
   <si>
     <t>MCR10HJ120</t>
+  </si>
+  <si>
+    <t>MMBT2222A</t>
+  </si>
+  <si>
+    <t>Diodes Inc</t>
+  </si>
+  <si>
+    <t>NPN transistor</t>
+  </si>
+  <si>
+    <t>MMBT2222A-FDICT-ND</t>
+  </si>
+  <si>
+    <t>VH enable</t>
+  </si>
+  <si>
+    <t>Vdd enable</t>
+  </si>
+  <si>
+    <t>Motor driver fault HEAD</t>
+  </si>
+  <si>
+    <t>Motor driver fault CUT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="g"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1151,7 +1180,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1183,9 +1212,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1217,6 +1247,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1392,14 +1423,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" customWidth="1"/>
     <col min="2" max="2" width="4.5703125" bestFit="1" customWidth="1"/>
@@ -1416,7 +1447,7 @@
     <col min="13" max="13" width="62.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1426,7 +1457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1437,27 +1468,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1498,7 +1529,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -1525,7 +1556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -1552,7 +1583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>3</v>
       </c>
@@ -1591,7 +1622,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>4</v>
       </c>
@@ -1630,7 +1661,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>5</v>
       </c>
@@ -1659,7 +1690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>6</v>
       </c>
@@ -1699,7 +1730,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>7</v>
       </c>
@@ -1717,7 +1748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>8</v>
       </c>
@@ -1735,7 +1766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>9</v>
       </c>
@@ -1753,16 +1784,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>10</v>
       </c>
+      <c r="E18" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="I18" t="s">
+        <v>35</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="K18" s="6">
+        <v>0.14000000000000001</v>
+      </c>
       <c r="L18" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>11</v>
       </c>
@@ -1792,7 +1841,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>12</v>
       </c>
@@ -1801,7 +1850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>13</v>
       </c>
@@ -1810,7 +1859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>14</v>
       </c>
@@ -1819,7 +1868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>15</v>
       </c>
@@ -1828,7 +1877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>16</v>
       </c>
@@ -1837,7 +1886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>17</v>
       </c>
@@ -1858,7 +1907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>18</v>
       </c>
@@ -1882,7 +1931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>19</v>
       </c>
@@ -1906,7 +1955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>20</v>
       </c>
@@ -1930,7 +1979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>21</v>
       </c>
@@ -1954,7 +2003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>22</v>
       </c>
@@ -1963,7 +2012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>23</v>
       </c>
@@ -1987,7 +2036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>24</v>
       </c>
@@ -2011,7 +2060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>25</v>
       </c>
@@ -2031,7 +2080,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>26</v>
       </c>
@@ -2051,7 +2100,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>27</v>
       </c>
@@ -2071,7 +2120,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>28</v>
       </c>
@@ -2091,7 +2140,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>29</v>
       </c>
@@ -2111,12 +2160,12 @@
         <v>233</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>31</v>
       </c>
@@ -2127,22 +2176,22 @@
         <v>240</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>25</v>
       </c>
@@ -2186,21 +2235,22 @@
     <hyperlink ref="J14" r:id="rId4"/>
     <hyperlink ref="G19" r:id="rId5" display="https://www.onsemi.com/PowerSolutions/product.do?id=CAT24C256WI-GT3"/>
     <hyperlink ref="J19" r:id="rId6"/>
+    <hyperlink ref="J18" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" customWidth="1"/>
     <col min="3" max="3" width="3.85546875" bestFit="1" customWidth="1"/>
@@ -2209,12 +2259,12 @@
     <col min="8" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -2234,7 +2284,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -2257,7 +2307,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -2280,7 +2330,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -2299,7 +2349,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -2328,7 +2378,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -2357,7 +2407,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>6</v>
       </c>
@@ -2376,17 +2426,8 @@
       <c r="F9" t="s">
         <v>103</v>
       </c>
-      <c r="H9" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="I9" t="s">
-        <v>147</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>7</v>
       </c>
@@ -2406,7 +2447,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>8</v>
       </c>
@@ -2425,8 +2466,20 @@
       <c r="F11" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="G11" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="I11" t="s">
+        <v>147</v>
+      </c>
+      <c r="J11" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>9</v>
       </c>
@@ -2451,11 +2504,11 @@
       <c r="I12" t="s">
         <v>148</v>
       </c>
-      <c r="J12" s="10" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="J12" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>10</v>
       </c>
@@ -2480,8 +2533,11 @@
       <c r="I13" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="J13" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>11</v>
       </c>
@@ -2506,8 +2562,11 @@
       <c r="I14" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="J14" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>12</v>
       </c>
@@ -2532,8 +2591,11 @@
       <c r="I15" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="J15" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>13</v>
       </c>
@@ -2553,7 +2615,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>14</v>
       </c>
@@ -2569,7 +2631,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>15</v>
       </c>
@@ -2585,7 +2647,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>16</v>
       </c>
@@ -2605,7 +2667,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>17</v>
       </c>
@@ -2625,7 +2687,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>18</v>
       </c>
@@ -2645,7 +2707,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>19</v>
       </c>
@@ -2665,7 +2727,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>20</v>
       </c>
@@ -2685,7 +2747,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>21</v>
       </c>
@@ -2705,7 +2767,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>22</v>
       </c>
@@ -2725,7 +2787,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>23</v>
       </c>
@@ -2745,7 +2807,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>24</v>
       </c>
@@ -2765,7 +2827,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>25</v>
       </c>
@@ -2783,7 +2845,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>26</v>
       </c>
@@ -2799,7 +2861,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>27</v>
       </c>
@@ -2819,7 +2881,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>28</v>
       </c>
@@ -2839,7 +2901,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>29</v>
       </c>
@@ -2859,7 +2921,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
         <v>30</v>
       </c>
@@ -2879,7 +2941,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <v>1</v>
       </c>
@@ -2902,7 +2964,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>2</v>
       </c>
@@ -2919,7 +2981,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <v>3</v>
       </c>
@@ -2942,7 +3004,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <v>4</v>
       </c>
@@ -2962,7 +3024,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <v>5</v>
       </c>
@@ -2982,7 +3044,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
         <v>6</v>
       </c>
@@ -3002,7 +3064,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>7</v>
       </c>
@@ -3022,7 +3084,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
         <v>8</v>
       </c>
@@ -3033,7 +3095,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>6</v>
       </c>
@@ -3044,7 +3106,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>3</v>
       </c>
@@ -3055,7 +3117,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>4</v>
       </c>
@@ -3066,7 +3128,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>4</v>
       </c>
@@ -3077,7 +3139,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1</v>
       </c>
@@ -3088,7 +3150,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2</v>
       </c>
@@ -3099,7 +3161,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2</v>
       </c>
@@ -3110,7 +3172,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1</v>
       </c>
@@ -3121,7 +3183,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <f>SUM(A47:A52)</f>
         <v>20</v>
@@ -3133,24 +3195,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="12" max="12" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -3182,7 +3244,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -3214,7 +3276,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -3249,7 +3311,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -3284,7 +3346,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -3316,7 +3378,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -3348,7 +3410,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>6</v>
       </c>
@@ -3380,7 +3442,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>7</v>
       </c>
@@ -3409,7 +3471,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>8</v>
       </c>
@@ -3441,7 +3503,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>9</v>
       </c>
@@ -3473,7 +3535,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>10</v>
       </c>
@@ -3505,7 +3567,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>11</v>
       </c>
@@ -3537,7 +3599,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>12</v>
       </c>
@@ -3569,7 +3631,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>13</v>
       </c>
@@ -3601,7 +3663,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>14</v>
       </c>
@@ -3633,7 +3695,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>15</v>
       </c>
@@ -3662,7 +3724,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>16</v>
       </c>
@@ -3694,7 +3756,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>17</v>
       </c>
@@ -3726,7 +3788,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>18</v>
       </c>
@@ -3758,7 +3820,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>19</v>
       </c>
@@ -3790,7 +3852,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>20</v>
       </c>
@@ -3822,7 +3884,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>21</v>
       </c>
@@ -3854,7 +3916,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>22</v>
       </c>
@@ -3886,7 +3948,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>23</v>
       </c>
@@ -3918,7 +3980,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>24</v>
       </c>
@@ -3950,7 +4012,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>25</v>
       </c>
@@ -3979,7 +4041,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>26</v>
       </c>
@@ -4011,7 +4073,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>27</v>
       </c>
@@ -4043,7 +4105,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>28</v>
       </c>
@@ -4075,7 +4137,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>29</v>
       </c>
@@ -4107,7 +4169,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
         <v>30</v>
       </c>
@@ -4139,7 +4201,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <v>1</v>
       </c>
@@ -4171,7 +4233,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>2</v>
       </c>
@@ -4194,7 +4256,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <v>3</v>
       </c>
@@ -4217,7 +4279,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <v>4</v>
       </c>
@@ -4246,7 +4308,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <v>5</v>
       </c>
@@ -4275,7 +4337,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
         <v>6</v>
       </c>
@@ -4304,7 +4366,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>7</v>
       </c>
@@ -4333,7 +4395,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
         <v>8</v>
       </c>
@@ -4357,16 +4419,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>255</v>
       </c>
@@ -4395,7 +4457,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4424,7 +4486,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4453,7 +4515,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -4482,7 +4544,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -4511,7 +4573,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -4540,7 +4602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -4569,7 +4631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -4598,7 +4660,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -4627,7 +4689,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
         <v>93</v>
       </c>
@@ -4641,7 +4703,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -4670,7 +4732,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -4699,7 +4761,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -4728,7 +4790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Added sw and updated with latest design files. Updated README
</commit_message>
<xml_diff>
--- a/docs/TPCape_RevA_BOM.xlsx
+++ b/docs/TPCape_RevA_BOM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\thermal-printer\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\pru-printer\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="5970" windowHeight="5670" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="5970" windowHeight="5670" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TPcape_BOM" sheetId="4" r:id="rId1"/>
@@ -17,12 +17,12 @@
     <sheet name="interface" sheetId="6" r:id="rId3"/>
     <sheet name="motor" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511" iterate="1" iterateCount="10000"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="324">
   <si>
     <t>Capture CIS Standard Bill Of Materials - Standard Report</t>
   </si>
@@ -582,9 +582,6 @@
     <t>VDD_5V</t>
   </si>
   <si>
-    <t>Tpcape</t>
-  </si>
-  <si>
     <t>Vcc2</t>
   </si>
   <si>
@@ -948,16 +945,55 @@
     <t>MMBT2222A-FDICT-ND</t>
   </si>
   <si>
-    <t>VH enable</t>
-  </si>
-  <si>
-    <t>Vdd enable</t>
-  </si>
-  <si>
     <t>Motor driver fault HEAD</t>
   </si>
   <si>
     <t>Motor driver fault CUT</t>
+  </si>
+  <si>
+    <t>Vdd supply enable</t>
+  </si>
+  <si>
+    <t>VH supply enable</t>
+  </si>
+  <si>
+    <t>MTA_cut</t>
+  </si>
+  <si>
+    <t>MTAn_cut</t>
+  </si>
+  <si>
+    <t>MTB_cut</t>
+  </si>
+  <si>
+    <t>MTBn_cut</t>
+  </si>
+  <si>
+    <t>MTAn_head</t>
+  </si>
+  <si>
+    <t>MTA_head</t>
+  </si>
+  <si>
+    <t>MTBn_head</t>
+  </si>
+  <si>
+    <t>MTB_head</t>
+  </si>
+  <si>
+    <t>PRU Signal</t>
+  </si>
+  <si>
+    <t>Cape Signal</t>
+  </si>
+  <si>
+    <t>Interface board</t>
+  </si>
+  <si>
+    <t>Translation?</t>
+  </si>
+  <si>
+    <t>TPcape</t>
   </si>
 </sst>
 </file>
@@ -1426,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1789,19 +1825,19 @@
         <v>10</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I18" t="s">
         <v>35</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="K18" s="6">
         <v>0.14000000000000001</v>
@@ -1819,19 +1855,19 @@
         <v>1</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I19" t="s">
         <v>35</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K19" s="6">
         <v>0.73</v>
@@ -1891,16 +1927,16 @@
         <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D25" t="s">
+        <v>293</v>
+      </c>
+      <c r="E25" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="E25" s="13" t="s">
-        <v>295</v>
-      </c>
       <c r="G25" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L25" s="6">
         <f t="shared" si="0"/>
@@ -1912,19 +1948,19 @@
         <v>18</v>
       </c>
       <c r="C26" t="s">
+        <v>270</v>
+      </c>
+      <c r="D26" t="s">
+        <v>275</v>
+      </c>
+      <c r="E26" t="s">
+        <v>276</v>
+      </c>
+      <c r="F26" t="s">
+        <v>272</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>271</v>
-      </c>
-      <c r="D26" t="s">
-        <v>276</v>
-      </c>
-      <c r="E26" t="s">
-        <v>277</v>
-      </c>
-      <c r="F26" t="s">
-        <v>273</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>272</v>
       </c>
       <c r="L26" s="6">
         <f t="shared" si="0"/>
@@ -1936,19 +1972,19 @@
         <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D27" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E27" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F27" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L27" s="6">
         <f t="shared" si="0"/>
@@ -1960,19 +1996,19 @@
         <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D28" t="s">
+        <v>221</v>
+      </c>
+      <c r="E28" t="s">
         <v>222</v>
       </c>
-      <c r="E28" t="s">
-        <v>223</v>
-      </c>
       <c r="F28" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="L28" s="6">
         <f t="shared" si="0"/>
@@ -1984,19 +2020,19 @@
         <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D29" t="s">
+        <v>246</v>
+      </c>
+      <c r="E29" t="s">
         <v>247</v>
       </c>
-      <c r="E29" t="s">
-        <v>248</v>
-      </c>
       <c r="F29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L29" s="6">
         <f t="shared" si="0"/>
@@ -2017,19 +2053,19 @@
         <v>23</v>
       </c>
       <c r="C31" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D31">
         <v>12</v>
       </c>
       <c r="E31" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F31" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="L31" s="6">
         <f t="shared" si="0"/>
@@ -2041,19 +2077,19 @@
         <v>24</v>
       </c>
       <c r="C32" t="s">
+        <v>235</v>
+      </c>
+      <c r="D32" t="s">
+        <v>249</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="F32" t="s">
+        <v>241</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>236</v>
-      </c>
-      <c r="D32" t="s">
-        <v>250</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="F32" t="s">
-        <v>242</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>237</v>
       </c>
       <c r="L32" s="6">
         <f t="shared" si="0"/>
@@ -2065,19 +2101,19 @@
         <v>25</v>
       </c>
       <c r="C33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D33" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F33" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -2085,19 +2121,19 @@
         <v>26</v>
       </c>
       <c r="C34" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D34" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E34" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F34" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -2105,19 +2141,19 @@
         <v>27</v>
       </c>
       <c r="C35" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D35" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E35" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F35" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2125,19 +2161,19 @@
         <v>28</v>
       </c>
       <c r="C36" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D36">
         <v>180</v>
       </c>
       <c r="E36" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F36" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2145,19 +2181,19 @@
         <v>29</v>
       </c>
       <c r="C37" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D37" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F37" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2170,10 +2206,10 @@
         <v>31</v>
       </c>
       <c r="C39" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -2246,8 +2282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10:J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2257,6 +2293,7 @@
     <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="45.7109375" customWidth="1"/>
     <col min="8" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2327,7 +2364,7 @@
         <v>100</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2375,7 +2412,7 @@
         <v>138</v>
       </c>
       <c r="J7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2404,7 +2441,7 @@
         <v>158</v>
       </c>
       <c r="J8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -2446,6 +2483,15 @@
       <c r="F10" t="s">
         <v>104</v>
       </c>
+      <c r="H10" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
@@ -2467,7 +2513,7 @@
         <v>105</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>174</v>
@@ -2505,7 +2551,7 @@
         <v>148</v>
       </c>
       <c r="J12" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -2534,7 +2580,7 @@
         <v>149</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2563,7 +2609,7 @@
         <v>159</v>
       </c>
       <c r="J14" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2592,7 +2638,7 @@
         <v>161</v>
       </c>
       <c r="J15" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2614,8 +2660,17 @@
       <c r="F16" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H16" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="I16" t="s">
+        <v>140</v>
+      </c>
+      <c r="J16" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>14</v>
       </c>
@@ -2630,8 +2685,17 @@
       <c r="F17" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H17" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="I17" t="s">
+        <v>139</v>
+      </c>
+      <c r="J17" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>15</v>
       </c>
@@ -2646,8 +2710,17 @@
       <c r="F18" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H18" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="I18" t="s">
+        <v>141</v>
+      </c>
+      <c r="J18" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>16</v>
       </c>
@@ -2666,8 +2739,17 @@
       <c r="F19" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H19" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="I19" t="s">
+        <v>142</v>
+      </c>
+      <c r="J19" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>17</v>
       </c>
@@ -2686,8 +2768,17 @@
       <c r="F20" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H20" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="I20" t="s">
+        <v>143</v>
+      </c>
+      <c r="J20" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>18</v>
       </c>
@@ -2706,8 +2797,17 @@
       <c r="F21" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H21" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="I21" t="s">
+        <v>144</v>
+      </c>
+      <c r="J21" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>19</v>
       </c>
@@ -2726,8 +2826,17 @@
       <c r="F22" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H22" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="I22" t="s">
+        <v>145</v>
+      </c>
+      <c r="J22" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>20</v>
       </c>
@@ -2746,8 +2855,17 @@
       <c r="F23" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H23" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="I23" t="s">
+        <v>146</v>
+      </c>
+      <c r="J23" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>21</v>
       </c>
@@ -2766,8 +2884,17 @@
       <c r="F24" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H24" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="I24" t="s">
+        <v>135</v>
+      </c>
+      <c r="J24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>22</v>
       </c>
@@ -2786,8 +2913,17 @@
       <c r="F25" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H25" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="I25" t="s">
+        <v>136</v>
+      </c>
+      <c r="J25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>23</v>
       </c>
@@ -2806,8 +2942,17 @@
       <c r="F26" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H26" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="I26" t="s">
+        <v>134</v>
+      </c>
+      <c r="J26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>24</v>
       </c>
@@ -2826,8 +2971,17 @@
       <c r="F27" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H27" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="I27" t="s">
+        <v>133</v>
+      </c>
+      <c r="J27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>25</v>
       </c>
@@ -2844,8 +2998,17 @@
       <c r="F28" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H28" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="I28" t="s">
+        <v>130</v>
+      </c>
+      <c r="J28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>26</v>
       </c>
@@ -2860,8 +3023,17 @@
       <c r="F29" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H29" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="I29" t="s">
+        <v>131</v>
+      </c>
+      <c r="J29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>27</v>
       </c>
@@ -2880,8 +3052,17 @@
       <c r="F30" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H30" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="I30" t="s">
+        <v>137</v>
+      </c>
+      <c r="J30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>28</v>
       </c>
@@ -2900,8 +3081,17 @@
       <c r="F31" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H31" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="I31" t="s">
+        <v>132</v>
+      </c>
+      <c r="J31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>29</v>
       </c>
@@ -2920,8 +3110,17 @@
       <c r="F32" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H32" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="I32" t="s">
+        <v>129</v>
+      </c>
+      <c r="J32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
         <v>30</v>
       </c>
@@ -2940,8 +3139,17 @@
       <c r="F33" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H33" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="I33" t="s">
+        <v>160</v>
+      </c>
+      <c r="J33" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <v>1</v>
       </c>
@@ -2961,10 +3169,10 @@
         <v>122</v>
       </c>
       <c r="H36" s="10" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>2</v>
       </c>
@@ -2981,7 +3189,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <v>3</v>
       </c>
@@ -3004,7 +3212,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <v>4</v>
       </c>
@@ -3024,7 +3232,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <v>5</v>
       </c>
@@ -3044,7 +3252,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
         <v>6</v>
       </c>
@@ -3064,7 +3272,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>7</v>
       </c>
@@ -3084,7 +3292,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
         <v>8</v>
       </c>
@@ -3095,26 +3303,26 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>6</v>
       </c>
       <c r="B47" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E47" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>3</v>
       </c>
       <c r="B48" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E48" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -3122,10 +3330,10 @@
         <v>4</v>
       </c>
       <c r="B49" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E49" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3133,10 +3341,10 @@
         <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E50" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3144,10 +3352,10 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E51" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -3155,10 +3363,10 @@
         <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E52" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -3166,10 +3374,10 @@
         <v>2</v>
       </c>
       <c r="B53" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E53" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -3177,10 +3385,10 @@
         <v>1</v>
       </c>
       <c r="B54" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E54" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -3198,9 +3406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3208,8 +3414,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>186</v>
+      <c r="A2" t="s">
+        <v>323</v>
+      </c>
+      <c r="E2" t="s">
+        <v>322</v>
+      </c>
+      <c r="I2" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -3219,7 +3431,7 @@
       <c r="B3" t="s">
         <v>69</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="8" t="s">
         <v>70</v>
       </c>
       <c r="E3" t="s">
@@ -3228,7 +3440,7 @@
       <c r="F3" t="s">
         <v>69</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="8" t="s">
         <v>70</v>
       </c>
       <c r="I3" t="s">
@@ -3237,7 +3449,7 @@
       <c r="J3" t="s">
         <v>69</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="8" t="s">
         <v>70</v>
       </c>
       <c r="L3" t="s">
@@ -3258,22 +3470,22 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>195</v>
-      </c>
-      <c r="G4" t="s">
+        <v>194</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>96</v>
       </c>
       <c r="I4" s="9">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>195</v>
-      </c>
-      <c r="K4" t="s">
+        <v>194</v>
+      </c>
+      <c r="K4" s="8" t="s">
         <v>96</v>
       </c>
       <c r="L4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -3290,25 +3502,25 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>187</v>
-      </c>
-      <c r="G5" t="s">
+        <v>186</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I5" s="9">
         <v>2</v>
       </c>
       <c r="J5" t="s">
-        <v>187</v>
-      </c>
-      <c r="K5" t="s">
+        <v>186</v>
+      </c>
+      <c r="K5" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -3325,25 +3537,25 @@
         <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>188</v>
-      </c>
-      <c r="G6" t="s">
+        <v>187</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>98</v>
       </c>
       <c r="I6" s="9">
         <v>3</v>
       </c>
       <c r="J6" t="s">
-        <v>188</v>
-      </c>
-      <c r="K6" t="s">
+        <v>187</v>
+      </c>
+      <c r="K6" s="8" t="s">
         <v>98</v>
       </c>
       <c r="L6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -3362,20 +3574,20 @@
       <c r="F7" t="s">
         <v>77</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I7" s="9">
         <v>4</v>
       </c>
       <c r="J7" t="s">
-        <v>189</v>
-      </c>
-      <c r="K7" t="s">
+        <v>188</v>
+      </c>
+      <c r="K7" s="8" t="s">
         <v>98</v>
       </c>
       <c r="L7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -3394,20 +3606,20 @@
       <c r="F8" t="s">
         <v>77</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I8" s="9">
         <v>5</v>
       </c>
       <c r="J8" t="s">
-        <v>190</v>
-      </c>
-      <c r="K8" t="s">
+        <v>189</v>
+      </c>
+      <c r="K8" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -3424,9 +3636,9 @@
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>191</v>
-      </c>
-      <c r="G9" t="s">
+        <v>190</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I9" s="9">
@@ -3435,11 +3647,11 @@
       <c r="J9" t="s">
         <v>77</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -3456,9 +3668,9 @@
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>192</v>
-      </c>
-      <c r="G10" t="s">
+        <v>191</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I10" s="9">
@@ -3467,7 +3679,7 @@
       <c r="J10" t="s">
         <v>77</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="8" t="s">
         <v>97</v>
       </c>
     </row>
@@ -3487,20 +3699,20 @@
       <c r="F11" t="s">
         <v>80</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="8" t="s">
         <v>96</v>
       </c>
       <c r="I11" s="9">
         <v>8</v>
       </c>
       <c r="J11" t="s">
-        <v>191</v>
-      </c>
-      <c r="K11" t="s">
+        <v>190</v>
+      </c>
+      <c r="K11" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -3519,20 +3731,20 @@
       <c r="F12" t="s">
         <v>80</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="8" t="s">
         <v>96</v>
       </c>
       <c r="I12" s="9">
         <v>9</v>
       </c>
       <c r="J12" t="s">
-        <v>192</v>
-      </c>
-      <c r="K12" t="s">
+        <v>191</v>
+      </c>
+      <c r="K12" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -3551,7 +3763,7 @@
       <c r="F13" t="s">
         <v>81</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I13" s="9">
@@ -3560,11 +3772,11 @@
       <c r="J13" t="s">
         <v>80</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="8" t="s">
         <v>96</v>
       </c>
       <c r="L13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -3583,7 +3795,7 @@
       <c r="F14" t="s">
         <v>82</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I14" s="9">
@@ -3592,11 +3804,11 @@
       <c r="J14" t="s">
         <v>80</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="8" t="s">
         <v>96</v>
       </c>
       <c r="L14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -3615,7 +3827,7 @@
       <c r="F15" t="s">
         <v>83</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I15" s="9">
@@ -3624,11 +3836,11 @@
       <c r="J15" t="s">
         <v>81</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K15" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -3645,9 +3857,9 @@
         <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>190</v>
-      </c>
-      <c r="G16" t="s">
+        <v>189</v>
+      </c>
+      <c r="G16" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I16" s="9">
@@ -3656,11 +3868,11 @@
       <c r="J16" t="s">
         <v>82</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -3677,7 +3889,7 @@
         <v>16</v>
       </c>
       <c r="F17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>98</v>
@@ -3688,11 +3900,11 @@
       <c r="J17" t="s">
         <v>83</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -3709,18 +3921,18 @@
         <v>17</v>
       </c>
       <c r="F18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I18" s="9">
         <v>15</v>
       </c>
       <c r="J18" t="s">
-        <v>190</v>
-      </c>
-      <c r="K18" t="s">
+        <v>189</v>
+      </c>
+      <c r="K18" s="8" t="s">
         <v>97</v>
       </c>
     </row>
@@ -3740,20 +3952,20 @@
       <c r="F19" t="s">
         <v>86</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I19" s="9">
         <v>16</v>
       </c>
       <c r="J19" t="s">
-        <v>300</v>
-      </c>
-      <c r="K19" t="s">
+        <v>299</v>
+      </c>
+      <c r="K19" s="8" t="s">
         <v>98</v>
       </c>
       <c r="L19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -3772,20 +3984,20 @@
       <c r="F20" t="s">
         <v>87</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I20" s="9">
         <v>17</v>
       </c>
       <c r="J20" t="s">
-        <v>193</v>
-      </c>
-      <c r="K20" t="s">
-        <v>301</v>
+        <v>192</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>300</v>
       </c>
       <c r="L20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -3804,7 +4016,7 @@
       <c r="F21" t="s">
         <v>88</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I21" s="9">
@@ -3813,11 +4025,11 @@
       <c r="J21" t="s">
         <v>86</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K21" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -3836,7 +4048,7 @@
       <c r="F22" t="s">
         <v>80</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="8" t="s">
         <v>96</v>
       </c>
       <c r="I22" s="9">
@@ -3845,11 +4057,11 @@
       <c r="J22" t="s">
         <v>87</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K22" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L22" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -3868,7 +4080,7 @@
       <c r="F23" t="s">
         <v>80</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="8" t="s">
         <v>96</v>
       </c>
       <c r="I23" s="9">
@@ -3877,11 +4089,11 @@
       <c r="J23" t="s">
         <v>88</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -3898,9 +4110,9 @@
         <v>23</v>
       </c>
       <c r="F24" t="s">
-        <v>194</v>
-      </c>
-      <c r="G24" t="s">
+        <v>193</v>
+      </c>
+      <c r="G24" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I24" s="9">
@@ -3909,11 +4121,11 @@
       <c r="J24" t="s">
         <v>80</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24" s="8" t="s">
         <v>96</v>
       </c>
       <c r="L24" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -3932,7 +4144,7 @@
       <c r="F25" t="s">
         <v>78</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="8" t="s">
         <v>98</v>
       </c>
       <c r="I25" s="9">
@@ -3941,11 +4153,11 @@
       <c r="J25" t="s">
         <v>80</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K25" s="8" t="s">
         <v>96</v>
       </c>
       <c r="L25" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -3964,20 +4176,20 @@
       <c r="F26" t="s">
         <v>77</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I26" s="9">
         <v>23</v>
       </c>
       <c r="J26" t="s">
-        <v>194</v>
-      </c>
-      <c r="K26" t="s">
+        <v>193</v>
+      </c>
+      <c r="K26" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -3996,7 +4208,7 @@
       <c r="F27" t="s">
         <v>77</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I27" s="9">
@@ -4005,11 +4217,11 @@
       <c r="J27" t="s">
         <v>78</v>
       </c>
-      <c r="K27" t="s">
+      <c r="K27" s="8" t="s">
         <v>98</v>
       </c>
       <c r="L27" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -4026,9 +4238,9 @@
         <v>5</v>
       </c>
       <c r="F28" t="s">
-        <v>190</v>
-      </c>
-      <c r="G28" t="s">
+        <v>189</v>
+      </c>
+      <c r="G28" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I28" s="9">
@@ -4037,7 +4249,7 @@
       <c r="J28" t="s">
         <v>77</v>
       </c>
-      <c r="K28" t="s">
+      <c r="K28" s="8" t="s">
         <v>97</v>
       </c>
     </row>
@@ -4055,9 +4267,9 @@
         <v>4</v>
       </c>
       <c r="F29" t="s">
-        <v>189</v>
-      </c>
-      <c r="G29" t="s">
+        <v>188</v>
+      </c>
+      <c r="G29" s="8" t="s">
         <v>98</v>
       </c>
       <c r="I29" s="9">
@@ -4066,11 +4278,11 @@
       <c r="J29" t="s">
         <v>77</v>
       </c>
-      <c r="K29" t="s">
+      <c r="K29" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L29" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -4089,7 +4301,7 @@
       <c r="F30" t="s">
         <v>92</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I30" s="9">
@@ -4098,11 +4310,11 @@
       <c r="J30" t="s">
         <v>92</v>
       </c>
-      <c r="K30" t="s">
+      <c r="K30" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L30" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -4121,7 +4333,7 @@
       <c r="F31" t="s">
         <v>93</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I31" s="9">
@@ -4130,11 +4342,11 @@
       <c r="J31" t="s">
         <v>93</v>
       </c>
-      <c r="K31" t="s">
+      <c r="K31" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L31" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -4153,7 +4365,7 @@
       <c r="F32" t="s">
         <v>94</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I32" s="9">
@@ -4162,11 +4374,11 @@
       <c r="J32" t="s">
         <v>94</v>
       </c>
-      <c r="K32" t="s">
+      <c r="K32" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L32" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -4185,7 +4397,7 @@
       <c r="F33" t="s">
         <v>95</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G33" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I33" s="9">
@@ -4194,12 +4406,20 @@
       <c r="J33" t="s">
         <v>95</v>
       </c>
-      <c r="K33" t="s">
+      <c r="K33" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L33" t="s">
-        <v>215</v>
-      </c>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G34" s="8"/>
+      <c r="K34" s="8"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G35" s="8"/>
+      <c r="K35" s="8"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
@@ -4215,22 +4435,22 @@
         <v>1</v>
       </c>
       <c r="F36" t="s">
-        <v>187</v>
-      </c>
-      <c r="G36" t="s">
+        <v>186</v>
+      </c>
+      <c r="G36" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I36" s="9">
         <v>1</v>
       </c>
       <c r="J36" t="s">
-        <v>187</v>
-      </c>
-      <c r="K36" t="s">
+        <v>186</v>
+      </c>
+      <c r="K36" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L36" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -4243,17 +4463,18 @@
       <c r="C37" s="9" t="s">
         <v>98</v>
       </c>
+      <c r="G37" s="8"/>
       <c r="I37" s="9">
         <v>2</v>
       </c>
       <c r="J37" t="s">
-        <v>196</v>
-      </c>
-      <c r="K37" t="s">
+        <v>195</v>
+      </c>
+      <c r="K37" s="8" t="s">
         <v>98</v>
       </c>
       <c r="L37" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -4266,17 +4487,18 @@
       <c r="C38" s="9" t="s">
         <v>96</v>
       </c>
+      <c r="G38" s="8"/>
       <c r="I38" s="9">
         <v>3</v>
       </c>
       <c r="J38" t="s">
-        <v>197</v>
-      </c>
-      <c r="K38" t="s">
+        <v>196</v>
+      </c>
+      <c r="K38" s="8" t="s">
         <v>98</v>
       </c>
       <c r="L38" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -4293,18 +4515,18 @@
         <v>4</v>
       </c>
       <c r="F39" t="s">
-        <v>198</v>
-      </c>
-      <c r="G39" t="s">
+        <v>197</v>
+      </c>
+      <c r="G39" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I39" s="9">
         <v>4</v>
       </c>
       <c r="J39" t="s">
-        <v>198</v>
-      </c>
-      <c r="K39" t="s">
+        <v>197</v>
+      </c>
+      <c r="K39" s="8" t="s">
         <v>97</v>
       </c>
     </row>
@@ -4322,18 +4544,18 @@
         <v>5</v>
       </c>
       <c r="F40" t="s">
-        <v>199</v>
-      </c>
-      <c r="G40" t="s">
+        <v>198</v>
+      </c>
+      <c r="G40" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I40" s="9">
         <v>5</v>
       </c>
       <c r="J40" t="s">
-        <v>199</v>
-      </c>
-      <c r="K40" t="s">
+        <v>198</v>
+      </c>
+      <c r="K40" s="8" t="s">
         <v>97</v>
       </c>
     </row>
@@ -4351,18 +4573,18 @@
         <v>6</v>
       </c>
       <c r="F41" t="s">
-        <v>200</v>
-      </c>
-      <c r="G41" t="s">
+        <v>199</v>
+      </c>
+      <c r="G41" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I41" s="9">
         <v>6</v>
       </c>
       <c r="J41" t="s">
-        <v>200</v>
-      </c>
-      <c r="K41" t="s">
+        <v>199</v>
+      </c>
+      <c r="K41" s="8" t="s">
         <v>97</v>
       </c>
     </row>
@@ -4380,18 +4602,18 @@
         <v>7</v>
       </c>
       <c r="F42" t="s">
-        <v>201</v>
-      </c>
-      <c r="G42" t="s">
+        <v>200</v>
+      </c>
+      <c r="G42" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I42" s="9">
         <v>7</v>
       </c>
       <c r="J42" t="s">
-        <v>201</v>
-      </c>
-      <c r="K42" t="s">
+        <v>200</v>
+      </c>
+      <c r="K42" s="8" t="s">
         <v>97</v>
       </c>
     </row>
@@ -4405,12 +4627,14 @@
       <c r="C43" s="9" t="s">
         <v>96</v>
       </c>
+      <c r="G43" s="8"/>
       <c r="I43" s="9">
         <v>8</v>
       </c>
       <c r="J43" t="s">
         <v>121</v>
       </c>
+      <c r="K43" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4422,39 +4646,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B1" t="s">
         <v>255</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>256</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>257</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>258</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>259</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>260</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>261</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>262</v>
-      </c>
-      <c r="K1" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>